<commit_message>
made a lot of modifications in the model_trainer
</commit_message>
<xml_diff>
--- a/trained_models/model1/saved_per_train/train2/Epoch40_loss0.69/saved_weights_biases.xlsx
+++ b/trained_models/model1/saved_per_train/train2/Epoch40_loss0.69/saved_weights_biases.xlsx
@@ -348,156 +348,156 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
-        <v>0.225991502404213</v>
+        <v>0.2218201011419296</v>
       </c>
       <c r="B1">
-        <v>0.8812246322631836</v>
+        <v>0.8797663450241089</v>
       </c>
       <c r="C1">
-        <v>0.3463990092277527</v>
+        <v>0.3352998793125153</v>
       </c>
       <c r="E1">
-        <v>0.04603033512830734</v>
+        <v>0.03339157998561859</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>-0.1395775824785233</v>
+        <v>-0.1414722353219986</v>
       </c>
       <c r="B2">
-        <v>0.5186605453491211</v>
+        <v>0.517657995223999</v>
       </c>
       <c r="C2">
-        <v>-0.1364690065383911</v>
+        <v>-0.1378511488437653</v>
       </c>
       <c r="E2">
-        <v>0.4714416265487671</v>
+        <v>0.4814306199550629</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>-0.3954614698886871</v>
+        <v>-0.3912558257579803</v>
       </c>
       <c r="B3">
-        <v>0.1323546469211578</v>
+        <v>0.123186931014061</v>
       </c>
       <c r="C3">
-        <v>0.5839434266090393</v>
+        <v>0.5839358568191528</v>
       </c>
       <c r="E3">
-        <v>0.3457987606525421</v>
+        <v>0.3432807326316833</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>-0.2660908102989197</v>
+        <v>-0.2614916861057281</v>
       </c>
       <c r="B6">
-        <v>0.02692349255084991</v>
+        <v>-0.005694939289242029</v>
       </c>
       <c r="C6">
-        <v>0.4565519392490387</v>
+        <v>0.4574137330055237</v>
       </c>
       <c r="E6">
-        <v>-0.05803164467215538</v>
+        <v>-0.06054602935910225</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>0.4851511418819427</v>
+        <v>0.4860560297966003</v>
       </c>
       <c r="B7">
-        <v>0.7804925441741943</v>
+        <v>0.7811156511306763</v>
       </c>
       <c r="C7">
-        <v>-0.04654132574796677</v>
+        <v>-0.04675938934087753</v>
       </c>
       <c r="E7">
-        <v>-0.1150888204574585</v>
+        <v>-0.1118023246526718</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>-0.001902673742733896</v>
+        <v>-0.001902643474750221</v>
       </c>
       <c r="B8">
-        <v>-9.736461834108923E-06</v>
+        <v>-9.703615432954393E-06</v>
       </c>
       <c r="C8">
-        <v>-2.538407954943978E-07</v>
+        <v>-2.115065740326827E-07</v>
       </c>
       <c r="E8">
-        <v>-0.009528292343020439</v>
+        <v>-0.008159401826560497</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>0.1080277860164642</v>
+        <v>0.1063886731863022</v>
       </c>
       <c r="B9">
-        <v>-0.4574795663356781</v>
+        <v>-0.4544883966445923</v>
       </c>
       <c r="C9">
-        <v>0.08351472020149231</v>
+        <v>0.08116413652896881</v>
       </c>
       <c r="E9">
-        <v>0.03993997350335121</v>
+        <v>0.03846239671111107</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>0.005963621195405722</v>
+        <v>0.005105503369122744</v>
       </c>
       <c r="B10">
-        <v>-0.08409331738948822</v>
+        <v>-0.09559169411659241</v>
       </c>
       <c r="C10">
-        <v>-0.1362041980028152</v>
+        <v>-0.1391779780387878</v>
       </c>
       <c r="E10">
-        <v>-0.001495533040724695</v>
+        <v>-0.007359105627983809</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>0.09010926634073257</v>
+        <v>0.08559130132198334</v>
       </c>
       <c r="B11">
-        <v>0.740622341632843</v>
+        <v>0.7200828194618225</v>
       </c>
       <c r="C11">
-        <v>-0.5477947592735291</v>
+        <v>-0.5547611117362976</v>
       </c>
       <c r="E11">
-        <v>0.0825478658080101</v>
+        <v>0.08132089674472809</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>0.3251109719276428</v>
+        <v>0.3275156617164612</v>
       </c>
       <c r="B12">
-        <v>-0.1879943013191223</v>
+        <v>-0.1929962188005447</v>
       </c>
       <c r="C12">
-        <v>-0.02826758846640587</v>
+        <v>-0.0313073918223381</v>
       </c>
       <c r="E12">
-        <v>-0.007756086532026529</v>
+        <v>-0.01871336624026299</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>-0.04027740657329559</v>
+        <v>-0.04027653113007545</v>
       </c>
       <c r="B13">
-        <v>3.232714152545668E-05</v>
+        <v>-1.889614850369981E-06</v>
       </c>
       <c r="C13">
-        <v>2.160663825634401E-06</v>
+        <v>4.673864168580621E-06</v>
       </c>
       <c r="E13">
-        <v>0.03732558712363243</v>
+        <v>0.04259041324257851</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -516,309 +516,309 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>0.2181510776281357</v>
+        <v>0.2169511020183563</v>
       </c>
       <c r="B15">
-        <v>0.2896229326725006</v>
+        <v>0.2880286276340485</v>
       </c>
       <c r="C15">
-        <v>0.04515621066093445</v>
+        <v>0.04734301939606667</v>
       </c>
       <c r="E15">
-        <v>0.1043002009391785</v>
+        <v>0.1053084656596184</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>0.001708047464489937</v>
+        <v>-0.01410045102238655</v>
       </c>
       <c r="B16">
-        <v>0.02163242734968662</v>
+        <v>0.05802565068006516</v>
       </c>
       <c r="C16">
-        <v>0.02493042312562466</v>
+        <v>0.02974939346313477</v>
       </c>
       <c r="E16">
-        <v>0.199661061167717</v>
+        <v>0.2804648876190186</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17">
-        <v>0.1664580255746841</v>
+        <v>0.1659751534461975</v>
       </c>
       <c r="B17">
-        <v>0.5199743509292603</v>
+        <v>0.5177063345909119</v>
       </c>
       <c r="C17">
-        <v>0.4297160506248474</v>
+        <v>0.4340869784355164</v>
       </c>
       <c r="E17">
-        <v>-0.06295337527990341</v>
+        <v>-0.06475374102592468</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18">
-        <v>-0.0184943899512291</v>
+        <v>-0.01498826500028372</v>
       </c>
       <c r="B18">
-        <v>0.0832052156329155</v>
+        <v>0.08552778512239456</v>
       </c>
       <c r="C18">
-        <v>0.04219989106059074</v>
+        <v>0.01942442171275616</v>
       </c>
       <c r="E18">
-        <v>0.1352803558111191</v>
+        <v>0.1534584611654282</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19">
-        <v>0.3599546551704407</v>
+        <v>0.361115425825119</v>
       </c>
       <c r="B19">
-        <v>-0.3265442252159119</v>
+        <v>-0.3159496486186981</v>
       </c>
       <c r="C19">
-        <v>-0.4084776341915131</v>
+        <v>-0.411693811416626</v>
       </c>
       <c r="E19">
-        <v>-0.02585859037935734</v>
+        <v>-0.01633981987833977</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20">
-        <v>-0.2694644331932068</v>
+        <v>-0.2758848071098328</v>
       </c>
       <c r="B20">
-        <v>0.007067206781357527</v>
+        <v>0.007837771438062191</v>
       </c>
       <c r="C20">
-        <v>0.3487516045570374</v>
+        <v>0.3435824811458588</v>
       </c>
       <c r="E20">
-        <v>0.1580961793661118</v>
+        <v>0.1510623544454575</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23">
-        <v>0.1262731701135635</v>
+        <v>0.1122782900929451</v>
       </c>
       <c r="B23">
-        <v>-0.08502160012722015</v>
+        <v>-0.08341693878173828</v>
       </c>
       <c r="C23">
-        <v>4.67788741076447E-09</v>
+        <v>5.397870239676195E-08</v>
       </c>
       <c r="D23">
-        <v>0.3333911895751953</v>
+        <v>0.3323299586772919</v>
       </c>
       <c r="E23">
-        <v>0.263264387845993</v>
+        <v>0.2664428353309631</v>
       </c>
       <c r="F23">
-        <v>-0.2831243574619293</v>
+        <v>-0.2831969559192657</v>
       </c>
       <c r="G23">
-        <v>0.05624810606241226</v>
+        <v>0.05713522061705589</v>
       </c>
       <c r="H23">
-        <v>0.0003141402557957917</v>
+        <v>0.0005621487507596612</v>
       </c>
       <c r="I23">
         <v>-6.390373482520758E-20</v>
       </c>
       <c r="J23">
-        <v>0.3376482129096985</v>
+        <v>0.3393676578998566</v>
       </c>
       <c r="K23">
-        <v>-0.009133654646575451</v>
+        <v>-0.001695605926215649</v>
       </c>
       <c r="L23">
-        <v>0.4188501238822937</v>
+        <v>0.4216940701007843</v>
       </c>
       <c r="M23">
-        <v>0.01418751571327448</v>
+        <v>0.01480967551469803</v>
       </c>
       <c r="N23">
-        <v>0.06458500027656555</v>
+        <v>0.06414780020713806</v>
       </c>
       <c r="O23">
-        <v>-0.01453621033579111</v>
+        <v>-0.02005638182163239</v>
       </c>
       <c r="Q23">
-        <v>0.003954904153943062</v>
+        <v>-0.001219142228364944</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24">
-        <v>0.2494328320026398</v>
+        <v>0.2545295655727386</v>
       </c>
       <c r="B24">
-        <v>-0.05761561915278435</v>
+        <v>-0.05253518745303154</v>
       </c>
       <c r="C24">
-        <v>2.303898099853541E-06</v>
+        <v>2.306238457094878E-06</v>
       </c>
       <c r="D24">
-        <v>0.05839097127318382</v>
+        <v>0.06428014487028122</v>
       </c>
       <c r="E24">
         <v>1.685708061599365E-18</v>
       </c>
       <c r="F24">
-        <v>-0.02071553468704224</v>
+        <v>-0.003450914984568954</v>
       </c>
       <c r="G24">
-        <v>-0.1168067753314972</v>
+        <v>-0.1117453053593636</v>
       </c>
       <c r="H24">
-        <v>0.0003179024206474423</v>
+        <v>0.0003328984312247485</v>
       </c>
       <c r="I24">
         <v>6.560578640346648E-07</v>
       </c>
       <c r="J24">
-        <v>-0.2572864592075348</v>
+        <v>-0.2515875101089478</v>
       </c>
       <c r="K24">
-        <v>-0.008911133743822575</v>
+        <v>-0.002977823838591576</v>
       </c>
       <c r="L24">
-        <v>0.2531945407390594</v>
+        <v>0.2582825422286987</v>
       </c>
       <c r="M24">
-        <v>0.001260085846297443</v>
+        <v>-0.00971820205450058</v>
       </c>
       <c r="N24">
-        <v>-0.09645518660545349</v>
+        <v>-0.09443928301334381</v>
       </c>
       <c r="O24">
-        <v>0.03406157344579697</v>
+        <v>0.03335342556238174</v>
       </c>
       <c r="Q24">
-        <v>0.1220215708017349</v>
+        <v>0.1314844489097595</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25">
-        <v>-0.2438423484563828</v>
+        <v>-0.2260558307170868</v>
       </c>
       <c r="B25">
-        <v>0.4555932581424713</v>
+        <v>0.4579233825206757</v>
       </c>
       <c r="C25">
-        <v>-1.220334979734616E-06</v>
+        <v>-1.229390250045981E-06</v>
       </c>
       <c r="D25">
-        <v>-0.1485393047332764</v>
+        <v>-0.1495067030191422</v>
       </c>
       <c r="E25">
-        <v>-0.2792621850967407</v>
+        <v>-0.2830626964569092</v>
       </c>
       <c r="F25">
-        <v>0.2441258728504181</v>
+        <v>0.2475768774747849</v>
       </c>
       <c r="G25">
-        <v>0.2238932251930237</v>
+        <v>0.2260856181383133</v>
       </c>
       <c r="H25">
-        <v>0.0007394395070150495</v>
+        <v>0.0008509393082931638</v>
       </c>
       <c r="I25">
         <v>1.981952379992435E-09</v>
       </c>
       <c r="J25">
-        <v>-0.2720584273338318</v>
+        <v>-0.269896000623703</v>
       </c>
       <c r="K25">
-        <v>0.02381055615842342</v>
+        <v>0.05871497839689255</v>
       </c>
       <c r="L25">
-        <v>0.124028280377388</v>
+        <v>0.1265635043382645</v>
       </c>
       <c r="M25">
-        <v>0.05215263366699219</v>
+        <v>0.07157766819000244</v>
       </c>
       <c r="N25">
-        <v>-0.3004624545574188</v>
+        <v>-0.2986831367015839</v>
       </c>
       <c r="O25">
-        <v>0.07638262957334518</v>
+        <v>0.08613719046115875</v>
       </c>
       <c r="Q25">
-        <v>0.04962737485766411</v>
+        <v>0.03806666657328606</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26">
-        <v>-0.3030383586883545</v>
+        <v>-0.303301990032196</v>
       </c>
       <c r="B26">
-        <v>0.190901905298233</v>
+        <v>0.1908273994922638</v>
       </c>
       <c r="C26">
-        <v>0.0001330964150838554</v>
+        <v>0.0001331718813162297</v>
       </c>
       <c r="D26">
-        <v>0.2886292636394501</v>
+        <v>0.2846396565437317</v>
       </c>
       <c r="E26">
-        <v>0.2735118567943573</v>
+        <v>0.280314028263092</v>
       </c>
       <c r="F26">
-        <v>0.04706498235464096</v>
+        <v>0.04809333011507988</v>
       </c>
       <c r="G26">
-        <v>0.2310348898172379</v>
+        <v>0.2312055677175522</v>
       </c>
       <c r="H26">
-        <v>-0.0005523215513676405</v>
+        <v>-0.0009723217808641493</v>
       </c>
       <c r="I26">
         <v>-5.610145308310166E-06</v>
       </c>
       <c r="J26">
-        <v>-0.06250450015068054</v>
+        <v>-0.06281612813472748</v>
       </c>
       <c r="K26">
-        <v>-0.01763620227575302</v>
+        <v>-0.07033660262823105</v>
       </c>
       <c r="L26">
-        <v>0.004685348831117153</v>
+        <v>0.00332177709788084</v>
       </c>
       <c r="M26">
-        <v>-0.04699713736772537</v>
+        <v>-0.0496477484703064</v>
       </c>
       <c r="N26">
-        <v>-0.2841325998306274</v>
+        <v>-0.2816865146160126</v>
       </c>
       <c r="O26">
-        <v>0.07048189640045166</v>
+        <v>0.07701320946216583</v>
       </c>
       <c r="Q26">
-        <v>0.02158693037927151</v>
+        <v>0.02123689465224743</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27">
-        <v>0.001251838984899223</v>
+        <v>0.0006734012858942151</v>
       </c>
       <c r="B27">
-        <v>-0.005374086555093527</v>
+        <v>-0.003900676500052214</v>
       </c>
       <c r="C27">
         <v>-1.367713196032128E-07</v>
       </c>
       <c r="D27">
-        <v>0.002517055254429579</v>
+        <v>0.002199471229687333</v>
       </c>
       <c r="E27">
-        <v>3.044112963834777E-05</v>
+        <v>6.720990495523438E-05</v>
       </c>
       <c r="F27">
-        <v>-0.009909005835652351</v>
+        <v>-0.0103355310857296</v>
       </c>
       <c r="G27">
-        <v>-0.002225280972197652</v>
+        <v>-0.002855187049135566</v>
       </c>
       <c r="H27">
         <v>-4.472505565900065E-07</v>
@@ -827,48 +827,48 @@
         <v>4.897719201569736E-17</v>
       </c>
       <c r="J27">
-        <v>-0.004216229543089867</v>
+        <v>-0.003151436801999807</v>
       </c>
       <c r="K27">
-        <v>-0.001103612245060503</v>
+        <v>5.063877324573696E-06</v>
       </c>
       <c r="L27">
-        <v>-0.00248602801002562</v>
+        <v>-0.001287821098230779</v>
       </c>
       <c r="M27">
-        <v>-6.822854174970416E-07</v>
+        <v>-4.837331601947881E-08</v>
       </c>
       <c r="N27">
-        <v>-0.009892087429761887</v>
+        <v>-0.01325591746717691</v>
       </c>
       <c r="O27">
-        <v>-1.736582999001257E-05</v>
+        <v>-1.806900399969891E-05</v>
       </c>
       <c r="Q27">
-        <v>-0.03075539693236351</v>
+        <v>-0.01888635754585266</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28">
-        <v>0.08465959876775742</v>
+        <v>0.09250794351100922</v>
       </c>
       <c r="B28">
-        <v>0.05829975381493568</v>
+        <v>0.06267771869897842</v>
       </c>
       <c r="C28">
         <v>-1.431655252885341E-19</v>
       </c>
       <c r="D28">
-        <v>-0.2681134939193726</v>
+        <v>-0.2673352062702179</v>
       </c>
       <c r="E28">
-        <v>0.1072001457214355</v>
+        <v>0.1049639210104942</v>
       </c>
       <c r="F28">
-        <v>-0.2493314892053604</v>
+        <v>-0.2392254173755646</v>
       </c>
       <c r="G28">
-        <v>0.3959891796112061</v>
+        <v>0.4011078774929047</v>
       </c>
       <c r="H28">
         <v>-1.45153876474069E-07</v>
@@ -877,39 +877,39 @@
         <v>1.828041095775813E-16</v>
       </c>
       <c r="J28">
-        <v>-0.175003707408905</v>
+        <v>-0.1710881143808365</v>
       </c>
       <c r="K28">
-        <v>0.005082285031676292</v>
+        <v>-0.04757494106888771</v>
       </c>
       <c r="L28">
-        <v>0.04661322757601738</v>
+        <v>0.0486939549446106</v>
       </c>
       <c r="M28">
-        <v>-0.06095695868134499</v>
+        <v>-0.02852027118206024</v>
       </c>
       <c r="N28">
-        <v>0.3805380463600159</v>
+        <v>0.3887678980827332</v>
       </c>
       <c r="O28">
-        <v>-0.12294752150774</v>
+        <v>-0.1237330362200737</v>
       </c>
       <c r="Q28">
-        <v>-0.0229693278670311</v>
+        <v>-0.02218468673527241</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29">
-        <v>-9.205404580825416E-07</v>
+        <v>-5.642201017508341E-07</v>
       </c>
       <c r="B29">
-        <v>-0.160128116607666</v>
+        <v>-0.1599052548408508</v>
       </c>
       <c r="C29">
         <v>-1.039346170728095E-05</v>
       </c>
       <c r="D29">
-        <v>2.722010322031565E-06</v>
+        <v>3.082931698372704E-06</v>
       </c>
       <c r="E29">
         <v>0.0003355448716320097</v>
@@ -918,7 +918,7 @@
         <v>6.295621801655216E-10</v>
       </c>
       <c r="G29">
-        <v>-0.07820583879947662</v>
+        <v>-0.07802937179803848</v>
       </c>
       <c r="H29">
         <v>-1.24109035937181E-07</v>
@@ -927,13 +927,13 @@
         <v>9.246431682270882E-19</v>
       </c>
       <c r="J29">
-        <v>0.1087684407830238</v>
+        <v>0.1089549958705902</v>
       </c>
       <c r="K29">
-        <v>-1.809567947930191E-06</v>
+        <v>-1.809660034268745E-06</v>
       </c>
       <c r="L29">
-        <v>0.02915710955858231</v>
+        <v>0.02964681200683117</v>
       </c>
       <c r="M29">
         <v>-4.811527105630375E-07</v>
@@ -942,60 +942,60 @@
         <v>6.716252300975611E-07</v>
       </c>
       <c r="O29">
-        <v>2.565313297964167E-05</v>
+        <v>2.650898386491463E-05</v>
       </c>
       <c r="Q29">
-        <v>-0.1169071570038795</v>
+        <v>-0.118207260966301</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30">
-        <v>0.02480329759418964</v>
+        <v>7.996116551112209E-07</v>
       </c>
       <c r="B30">
-        <v>-0.008592871949076653</v>
+        <v>-0.0004811654798686504</v>
       </c>
       <c r="C30">
-        <v>5.517154733070129E-09</v>
+        <v>4.365375372396537E-19</v>
       </c>
       <c r="D30">
-        <v>0.01888851821422577</v>
+        <v>6.240011884983687E-08</v>
       </c>
       <c r="E30">
-        <v>2.080908956259009E-07</v>
+        <v>5.1230797382118E-10</v>
       </c>
       <c r="F30">
-        <v>-0.0008795931935310364</v>
+        <v>1.085573307068872E-16</v>
       </c>
       <c r="G30">
-        <v>-0.02356140688061714</v>
+        <v>-0.0004414313589222729</v>
       </c>
       <c r="H30">
-        <v>3.294730959169101E-06</v>
+        <v>4.057713815363563E-20</v>
       </c>
       <c r="I30">
         <v>-5.238919584371615E-06</v>
       </c>
       <c r="J30">
-        <v>-0.00571034150198102</v>
+        <v>-2.863601366698276E-05</v>
       </c>
       <c r="K30">
-        <v>-0.003454624908044934</v>
+        <v>3.253894931276591E-07</v>
       </c>
       <c r="L30">
-        <v>0.0008370374562218785</v>
+        <v>-8.910299220588058E-05</v>
       </c>
       <c r="M30">
-        <v>-0.007365233264863491</v>
+        <v>-3.68515777893208E-08</v>
       </c>
       <c r="N30">
-        <v>-0.01600226014852524</v>
+        <v>-2.317375901839114E-06</v>
       </c>
       <c r="O30">
-        <v>0.005852058529853821</v>
+        <v>-5.867635763934231E-07</v>
       </c>
       <c r="Q30">
-        <v>-0.005593882873654366</v>
+        <v>-0.001895264605991542</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1050,25 +1050,25 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32">
-        <v>0.3276207447052002</v>
+        <v>0.3226787447929382</v>
       </c>
       <c r="B32">
-        <v>0.3587364852428436</v>
+        <v>0.360560417175293</v>
       </c>
       <c r="C32">
         <v>-5.727889699805867E-21</v>
       </c>
       <c r="D32">
-        <v>0.2732387185096741</v>
+        <v>0.2739845812320709</v>
       </c>
       <c r="E32">
-        <v>-0.2623518705368042</v>
+        <v>-0.2681123614311218</v>
       </c>
       <c r="F32">
-        <v>-0.1445463746786118</v>
+        <v>-0.1364343762397766</v>
       </c>
       <c r="G32">
-        <v>-0.06654650717973709</v>
+        <v>-0.0653223991394043</v>
       </c>
       <c r="H32">
         <v>9.394733524459298E-07</v>
@@ -1077,75 +1077,75 @@
         <v>-1.344190536656242E-09</v>
       </c>
       <c r="J32">
-        <v>-0.3628712296485901</v>
+        <v>-0.3612836301326752</v>
       </c>
       <c r="K32">
-        <v>0.01626452803611755</v>
+        <v>0.05073099583387375</v>
       </c>
       <c r="L32">
-        <v>0.03735017776489258</v>
+        <v>0.03860651329159737</v>
       </c>
       <c r="M32">
-        <v>0.03051597066223621</v>
+        <v>0.03930646926164627</v>
       </c>
       <c r="N32">
-        <v>0.2375347018241882</v>
+        <v>0.2387756854295731</v>
       </c>
       <c r="O32">
-        <v>0.2081253975629807</v>
+        <v>0.2205691635608673</v>
       </c>
       <c r="Q32">
-        <v>-0.1065409481525421</v>
+        <v>-0.1003137677907944</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33">
-        <v>0.3147047460079193</v>
+        <v>0.30487260222435</v>
       </c>
       <c r="B33">
-        <v>0.21024090051651</v>
+        <v>0.213935986161232</v>
       </c>
       <c r="C33">
-        <v>-2.183775471564786E-08</v>
+        <v>8.156430908456969E-08</v>
       </c>
       <c r="D33">
-        <v>-0.2413124144077301</v>
+        <v>-0.2434222996234894</v>
       </c>
       <c r="E33">
-        <v>0.2440294027328491</v>
+        <v>0.2372488677501678</v>
       </c>
       <c r="F33">
-        <v>-0.1275558620691299</v>
+        <v>-0.1250666975975037</v>
       </c>
       <c r="G33">
-        <v>-0.3838320374488831</v>
+        <v>-0.3805703222751617</v>
       </c>
       <c r="H33">
-        <v>-0.0002502643328625709</v>
+        <v>-0.0001056940527632833</v>
       </c>
       <c r="I33">
         <v>2.662634557282217E-09</v>
       </c>
       <c r="J33">
-        <v>0.007242823950946331</v>
+        <v>0.01080605387687683</v>
       </c>
       <c r="K33">
-        <v>0.005787331145256758</v>
+        <v>0.04162786900997162</v>
       </c>
       <c r="L33">
-        <v>0.2458718121051788</v>
+        <v>0.2487710565328598</v>
       </c>
       <c r="M33">
-        <v>0.05608953163027763</v>
+        <v>0.04118119180202484</v>
       </c>
       <c r="N33">
-        <v>-0.1519145965576172</v>
+        <v>-0.1484283804893494</v>
       </c>
       <c r="O33">
-        <v>0.2644064426422119</v>
+        <v>0.2637807130813599</v>
       </c>
       <c r="Q33">
-        <v>-0.13651143014431</v>
+        <v>-0.1302998214960098</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -1200,1102 +1200,1102 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35">
-        <v>-0.1586361229419708</v>
+        <v>-0.1689615398645401</v>
       </c>
       <c r="B35">
-        <v>-0.1658169627189636</v>
+        <v>-0.1698293089866638</v>
       </c>
       <c r="C35">
-        <v>5.862396210432053E-05</v>
+        <v>5.857885116711259E-05</v>
       </c>
       <c r="D35">
-        <v>0.05082414671778679</v>
+        <v>0.06048445031046867</v>
       </c>
       <c r="E35">
-        <v>-0.3230361342430115</v>
+        <v>-0.3162222504615784</v>
       </c>
       <c r="F35">
-        <v>-0.2433927357196808</v>
+        <v>-0.2564736008644104</v>
       </c>
       <c r="G35">
-        <v>0.3897694051265717</v>
+        <v>0.3863451182842255</v>
       </c>
       <c r="H35">
-        <v>-0.0001426443486707285</v>
+        <v>-0.000111811539682094</v>
       </c>
       <c r="I35">
         <v>0.0001991293393075466</v>
       </c>
       <c r="J35">
-        <v>0.4191066026687622</v>
+        <v>0.4151241481304169</v>
       </c>
       <c r="K35">
-        <v>0.008707333356142044</v>
+        <v>-0.01019176561385393</v>
       </c>
       <c r="L35">
-        <v>0.07747731357812881</v>
+        <v>0.07382439821958542</v>
       </c>
       <c r="M35">
-        <v>-0.01324257533997297</v>
+        <v>-0.006329250056296587</v>
       </c>
       <c r="N35">
-        <v>-0.2267614305019379</v>
+        <v>-0.227524146437645</v>
       </c>
       <c r="O35">
-        <v>0.001130331656895578</v>
+        <v>0.003573797410354018</v>
       </c>
       <c r="Q35">
-        <v>0.03660284727811813</v>
+        <v>0.03601808845996857</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36">
-        <v>-0.03447267040610313</v>
+        <v>-0.0422142967581749</v>
       </c>
       <c r="B36">
-        <v>0.2430875897407532</v>
+        <v>0.2393213212490082</v>
       </c>
       <c r="C36">
-        <v>1.475846147513948E-07</v>
+        <v>-1.390717443428002E-07</v>
       </c>
       <c r="D36">
-        <v>-0.4493478536605835</v>
+        <v>-0.4470280110836029</v>
       </c>
       <c r="E36">
-        <v>-0.08431653678417206</v>
+        <v>-0.07360422611236572</v>
       </c>
       <c r="F36">
-        <v>0.2540818452835083</v>
+        <v>0.2449362277984619</v>
       </c>
       <c r="G36">
-        <v>-0.1802405118942261</v>
+        <v>-0.1832819879055023</v>
       </c>
       <c r="H36">
-        <v>-0.0005701816407963634</v>
+        <v>-0.0006671578157693148</v>
       </c>
       <c r="I36">
         <v>3.459749677858781E-07</v>
       </c>
       <c r="J36">
-        <v>0.190301701426506</v>
+        <v>0.1867278963327408</v>
       </c>
       <c r="K36">
-        <v>-0.007429367862641811</v>
+        <v>-0.01567522250115871</v>
       </c>
       <c r="L36">
-        <v>0.09304014593362808</v>
+        <v>0.0889790952205658</v>
       </c>
       <c r="M36">
-        <v>0.0105135990306735</v>
+        <v>-0.01599620841443539</v>
       </c>
       <c r="N36">
-        <v>0.2212453484535217</v>
+        <v>0.2190329730510712</v>
       </c>
       <c r="O36">
-        <v>-0.01830553077161312</v>
+        <v>-0.01983344368636608</v>
       </c>
       <c r="Q36">
-        <v>0.02580054104328156</v>
+        <v>0.03139855340123177</v>
       </c>
     </row>
     <row r="37" spans="1:17">
       <c r="A37">
-        <v>0.1140648797154427</v>
+        <v>0.1332755982875824</v>
       </c>
       <c r="B37">
-        <v>-0.01726402528584003</v>
+        <v>-0.01549636851996183</v>
       </c>
       <c r="C37">
-        <v>-1.528044606402545E-07</v>
+        <v>1.543737937481637E-07</v>
       </c>
       <c r="D37">
-        <v>0.4572212994098663</v>
+        <v>0.4563295543193817</v>
       </c>
       <c r="E37">
-        <v>-0.2501539587974548</v>
+        <v>-0.2513065338134766</v>
       </c>
       <c r="F37">
-        <v>-0.007236675824970007</v>
+        <v>-0.004757838789373636</v>
       </c>
       <c r="G37">
-        <v>-0.3703954815864563</v>
+        <v>-0.3700249791145325</v>
       </c>
       <c r="H37">
-        <v>-0.0003336235240567476</v>
+        <v>-0.001006973325274885</v>
       </c>
       <c r="I37">
         <v>-1.430221914233698E-07</v>
       </c>
       <c r="J37">
-        <v>0.3875631988048553</v>
+        <v>0.3892439305782318</v>
       </c>
       <c r="K37">
-        <v>-0.01318445894867182</v>
+        <v>-0.04476700350642204</v>
       </c>
       <c r="L37">
-        <v>-0.06988722085952759</v>
+        <v>-0.06742002069950104</v>
       </c>
       <c r="M37">
-        <v>-0.02727396786212921</v>
+        <v>-0.009474274702370167</v>
       </c>
       <c r="N37">
-        <v>0.2576578259468079</v>
+        <v>0.2566614747047424</v>
       </c>
       <c r="O37">
-        <v>0.005977263208478689</v>
+        <v>0.001044959994032979</v>
       </c>
       <c r="Q37">
-        <v>0.1161285415291786</v>
+        <v>0.1154815107584</v>
       </c>
     </row>
     <row r="40" spans="1:17">
       <c r="A40">
-        <v>0.3290061950683594</v>
+        <v>0.3386206924915314</v>
       </c>
       <c r="B40">
-        <v>0.1235478445887566</v>
+        <v>0.1311642676591873</v>
       </c>
       <c r="C40">
-        <v>-0.1664560735225677</v>
+        <v>-0.1560770571231842</v>
       </c>
       <c r="D40">
-        <v>-0.3075056970119476</v>
+        <v>-0.2972297966480255</v>
       </c>
       <c r="E40">
-        <v>0.00103898230008781</v>
+        <v>0.0002590123331174254</v>
       </c>
       <c r="F40">
-        <v>-0.1968576610088348</v>
+        <v>-0.1896515786647797</v>
       </c>
       <c r="G40">
-        <v>-0.00710331043228507</v>
+        <v>-0.007094236090779305</v>
       </c>
       <c r="H40">
-        <v>-0.001637848792597651</v>
+        <v>-2.41292781311131E-08</v>
       </c>
       <c r="I40">
         <v>2.714569973250036E-06</v>
       </c>
       <c r="J40">
-        <v>-0.004090119153261185</v>
+        <v>0.003965700976550579</v>
       </c>
       <c r="K40">
-        <v>0.123370349407196</v>
+        <v>0.1385123282670975</v>
       </c>
       <c r="L40">
         <v>-1.798234450234304E-09</v>
       </c>
       <c r="M40">
-        <v>0.1543844193220139</v>
+        <v>0.1668704003095627</v>
       </c>
       <c r="N40">
-        <v>-0.1266034543514252</v>
+        <v>-0.1178919896483421</v>
       </c>
       <c r="O40">
-        <v>-0.02373507991433144</v>
+        <v>-0.0137668140232563</v>
       </c>
       <c r="Q40">
-        <v>0.1102058738470078</v>
+        <v>0.1403240859508514</v>
       </c>
     </row>
     <row r="41" spans="1:17">
       <c r="A41">
-        <v>-0.3778789937496185</v>
+        <v>-0.3780646622180939</v>
       </c>
       <c r="B41">
-        <v>-0.02065048553049564</v>
+        <v>-0.02193262241780758</v>
       </c>
       <c r="C41">
-        <v>0.3082069754600525</v>
+        <v>0.3058905005455017</v>
       </c>
       <c r="D41">
-        <v>-0.1150037422776222</v>
+        <v>-0.1166521683335304</v>
       </c>
       <c r="E41">
-        <v>0.01193780265748501</v>
+        <v>0.0144488075748086</v>
       </c>
       <c r="F41">
-        <v>0.201732411980629</v>
+        <v>0.2022785395383835</v>
       </c>
       <c r="G41">
         <v>-2.056538939143593E-08</v>
       </c>
       <c r="H41">
-        <v>-0.006711520720273256</v>
+        <v>-2.257663851423786E-07</v>
       </c>
       <c r="I41">
         <v>0.0003187915135640651</v>
       </c>
       <c r="J41">
-        <v>0.4284167289733887</v>
+        <v>0.4289373755455017</v>
       </c>
       <c r="K41">
-        <v>-0.02433355897665024</v>
+        <v>-0.0294102355837822</v>
       </c>
       <c r="L41">
         <v>-2.360387225053273E-05</v>
       </c>
       <c r="M41">
-        <v>0.006623677909374237</v>
+        <v>0.00753116887062788</v>
       </c>
       <c r="N41">
-        <v>0.2003151625394821</v>
+        <v>0.1972604542970657</v>
       </c>
       <c r="O41">
-        <v>-0.235478013753891</v>
+        <v>-0.23407843708992</v>
       </c>
       <c r="Q41">
-        <v>0.008514009416103363</v>
+        <v>0.008701899088919163</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42">
-        <v>0.02478131093084812</v>
+        <v>0.01974911242723465</v>
       </c>
       <c r="B42">
-        <v>0.01698336377739906</v>
+        <v>0.01444762758910656</v>
       </c>
       <c r="C42">
-        <v>-0.2842882573604584</v>
+        <v>-0.2858509719371796</v>
       </c>
       <c r="D42">
-        <v>0.328193873167038</v>
+        <v>0.3146346211433411</v>
       </c>
       <c r="E42">
-        <v>-0.0002223424380645156</v>
+        <v>4.855547012994066E-05</v>
       </c>
       <c r="F42">
-        <v>-0.2260445952415466</v>
+        <v>-0.2211017906665802</v>
       </c>
       <c r="G42">
-        <v>-0.001022374373860657</v>
+        <v>-0.001021780888549984</v>
       </c>
       <c r="H42">
-        <v>-0.0008574780076742172</v>
+        <v>-1.277237657859587E-07</v>
       </c>
       <c r="I42">
         <v>0.1684823483228683</v>
       </c>
       <c r="J42">
-        <v>0.07161468267440796</v>
+        <v>0.06752928346395493</v>
       </c>
       <c r="K42">
-        <v>0.2959076762199402</v>
+        <v>0.2879569828510284</v>
       </c>
       <c r="L42">
         <v>-2.277747412904318E-08</v>
       </c>
       <c r="M42">
-        <v>-0.08170245587825775</v>
+        <v>-0.08608634024858475</v>
       </c>
       <c r="N42">
-        <v>-0.1623619943857193</v>
+        <v>-0.162823498249054</v>
       </c>
       <c r="O42">
-        <v>0.1931235045194626</v>
+        <v>0.1762412339448929</v>
       </c>
       <c r="Q42">
-        <v>-0.02224984206259251</v>
+        <v>-0.02544179931282997</v>
       </c>
     </row>
     <row r="43" spans="1:17">
       <c r="A43">
-        <v>0.068319171667099</v>
+        <v>0.06899771094322205</v>
       </c>
       <c r="B43">
-        <v>0.04890751466155052</v>
+        <v>0.05346722528338432</v>
       </c>
       <c r="C43">
-        <v>-0.05248535796999931</v>
+        <v>-0.05338337272405624</v>
       </c>
       <c r="D43">
-        <v>0.3165681064128876</v>
+        <v>0.329576164484024</v>
       </c>
       <c r="E43">
-        <v>0.0002936614328064024</v>
+        <v>-0.005314538720995188</v>
       </c>
       <c r="F43">
-        <v>-0.2174272686243057</v>
+        <v>-0.2272926717996597</v>
       </c>
       <c r="G43">
-        <v>-6.274976840359159E-07</v>
+        <v>-6.218664339030511E-07</v>
       </c>
       <c r="H43">
-        <v>0.0004443419747985899</v>
+        <v>5.049144391477967E-08</v>
       </c>
       <c r="I43">
         <v>9.281564405938525E-10</v>
       </c>
       <c r="J43">
-        <v>-0.2384855300188065</v>
+        <v>-0.2497300505638123</v>
       </c>
       <c r="K43">
-        <v>0.2885378301143646</v>
+        <v>0.2990327179431915</v>
       </c>
       <c r="L43">
         <v>-1.271205363195804E-11</v>
       </c>
       <c r="M43">
-        <v>0.1617740094661713</v>
+        <v>0.1691816598176956</v>
       </c>
       <c r="N43">
-        <v>-0.4008095860481262</v>
+        <v>-0.4136874079704285</v>
       </c>
       <c r="O43">
-        <v>0.09148943424224854</v>
+        <v>0.11769849807024</v>
       </c>
       <c r="Q43">
-        <v>-0.1146518439054489</v>
+        <v>-0.1183974742889404</v>
       </c>
     </row>
     <row r="44" spans="1:17">
       <c r="A44">
-        <v>0.2850726842880249</v>
+        <v>0.2873709797859192</v>
       </c>
       <c r="B44">
-        <v>0.06859861314296722</v>
+        <v>0.07498546689748764</v>
       </c>
       <c r="C44">
-        <v>0.1759993731975555</v>
+        <v>0.1768857389688492</v>
       </c>
       <c r="D44">
-        <v>0.2704176306724548</v>
+        <v>0.272458404302597</v>
       </c>
       <c r="E44">
-        <v>0.004968416411429644</v>
+        <v>0.01239862944930792</v>
       </c>
       <c r="F44">
-        <v>-0.09256783872842789</v>
+        <v>-0.08913464844226837</v>
       </c>
       <c r="G44">
-        <v>3.069305421377067E-06</v>
+        <v>3.064196789637208E-06</v>
       </c>
       <c r="H44">
-        <v>0.007777566090226173</v>
+        <v>8.140204954543151E-07</v>
       </c>
       <c r="I44">
         <v>0.2768265604972839</v>
       </c>
       <c r="J44">
-        <v>-0.2427947521209717</v>
+        <v>-0.2399860322475433</v>
       </c>
       <c r="K44">
-        <v>0.1367281824350357</v>
+        <v>0.1395804882049561</v>
       </c>
       <c r="L44">
         <v>7.684185290178731E-19</v>
       </c>
       <c r="M44">
-        <v>0.233537346124649</v>
+        <v>0.2340002506971359</v>
       </c>
       <c r="N44">
-        <v>0.1621180325746536</v>
+        <v>0.1638685166835785</v>
       </c>
       <c r="O44">
-        <v>0.3820279240608215</v>
+        <v>0.3864531219005585</v>
       </c>
       <c r="Q44">
-        <v>0.1206754073500633</v>
+        <v>0.1194247901439667</v>
       </c>
     </row>
     <row r="45" spans="1:17">
       <c r="A45">
-        <v>0.2077530175447464</v>
+        <v>0.2069238126277924</v>
       </c>
       <c r="B45">
-        <v>-0.08121301233768463</v>
+        <v>-0.09055060893297195</v>
       </c>
       <c r="C45">
-        <v>0.2120356112718582</v>
+        <v>0.214694082736969</v>
       </c>
       <c r="D45">
-        <v>0.01886511221528053</v>
+        <v>0.01927695423364639</v>
       </c>
       <c r="E45">
-        <v>-0.001209082547575235</v>
+        <v>-0.01330383401364088</v>
       </c>
       <c r="F45">
-        <v>-0.4237932562828064</v>
+        <v>-0.4237250685691833</v>
       </c>
       <c r="G45">
-        <v>-0.004631168209016323</v>
+        <v>-0.00462478818371892</v>
       </c>
       <c r="H45">
-        <v>0.00427103228867054</v>
+        <v>-1.886199498812857E-07</v>
       </c>
       <c r="I45">
         <v>3.153999728056078E-08</v>
       </c>
       <c r="J45">
-        <v>-0.07305135577917099</v>
+        <v>-0.0733005702495575</v>
       </c>
       <c r="K45">
-        <v>0.5189816951751709</v>
+        <v>0.5102676153182983</v>
       </c>
       <c r="L45">
         <v>9.661653166403994E-06</v>
       </c>
       <c r="M45">
-        <v>0.293483555316925</v>
+        <v>0.2916825711727142</v>
       </c>
       <c r="N45">
-        <v>0.08496622741222382</v>
+        <v>0.08580208569765091</v>
       </c>
       <c r="O45">
-        <v>0.2592232823371887</v>
+        <v>0.2582500576972961</v>
       </c>
       <c r="Q45">
-        <v>-0.2614177763462067</v>
+        <v>-0.2554246485233307</v>
       </c>
     </row>
     <row r="46" spans="1:17">
       <c r="A46">
-        <v>0.08922086656093597</v>
+        <v>0.0993599146604538</v>
       </c>
       <c r="B46">
-        <v>-0.02511987276375294</v>
+        <v>-0.02270644716918468</v>
       </c>
       <c r="C46">
-        <v>-0.2104252576828003</v>
+        <v>-0.2247170954942703</v>
       </c>
       <c r="D46">
-        <v>-0.1633977144956589</v>
+        <v>-0.1772325187921524</v>
       </c>
       <c r="E46">
-        <v>-3.672846560220933E-06</v>
+        <v>-4.878101549365965E-07</v>
       </c>
       <c r="F46">
-        <v>-0.0904407724738121</v>
+        <v>-0.09590630233287811</v>
       </c>
       <c r="G46">
-        <v>-5.109062044539314E-07</v>
+        <v>-4.836112452721864E-07</v>
       </c>
       <c r="H46">
-        <v>-0.0001727945054881275</v>
+        <v>5.192199026282651E-08</v>
       </c>
       <c r="I46">
         <v>-0.1385851949453354</v>
       </c>
       <c r="J46">
-        <v>0.1080653220415115</v>
+        <v>0.1203637644648552</v>
       </c>
       <c r="K46">
-        <v>-0.1320870369672775</v>
+        <v>-0.1373720914125443</v>
       </c>
       <c r="L46">
         <v>-9.391892596966045E-09</v>
       </c>
       <c r="M46">
-        <v>0.1557203233242035</v>
+        <v>0.1632195562124252</v>
       </c>
       <c r="N46">
-        <v>-0.06599316000938416</v>
+        <v>-0.07001587003469467</v>
       </c>
       <c r="O46">
-        <v>0.267214298248291</v>
+        <v>0.2756727337837219</v>
       </c>
       <c r="Q46">
-        <v>-0.0473710261285305</v>
+        <v>-0.0397571437060833</v>
       </c>
     </row>
     <row r="47" spans="1:17">
       <c r="A47">
-        <v>-0.05725834891200066</v>
+        <v>-0.05428598076105118</v>
       </c>
       <c r="B47">
-        <v>0.1712397783994675</v>
+        <v>0.1593040525913239</v>
       </c>
       <c r="C47">
-        <v>-0.3712952136993408</v>
+        <v>-0.3604328632354736</v>
       </c>
       <c r="D47">
-        <v>0.1705048233270645</v>
+        <v>0.1778213381767273</v>
       </c>
       <c r="E47">
-        <v>0.02486158162355423</v>
+        <v>0.01579678431153297</v>
       </c>
       <c r="F47">
-        <v>0.2996254861354828</v>
+        <v>0.303098052740097</v>
       </c>
       <c r="G47">
-        <v>-0.02936168573796749</v>
+        <v>-0.02934827283024788</v>
       </c>
       <c r="H47">
-        <v>0.01711663044989109</v>
+        <v>-2.911139063144219E-06</v>
       </c>
       <c r="I47">
         <v>0.0658738911151886</v>
       </c>
       <c r="J47">
-        <v>0.3554926216602325</v>
+        <v>0.3603786528110504</v>
       </c>
       <c r="K47">
-        <v>0.3323160409927368</v>
+        <v>0.3407401442527771</v>
       </c>
       <c r="L47">
         <v>-1.393587328868406E-10</v>
       </c>
       <c r="M47">
-        <v>0.195110872387886</v>
+        <v>0.1923382133245468</v>
       </c>
       <c r="N47">
-        <v>-0.02946378104388714</v>
+        <v>-0.01812781020998955</v>
       </c>
       <c r="O47">
-        <v>-0.237214982509613</v>
+        <v>-0.2349926829338074</v>
       </c>
       <c r="Q47">
-        <v>-0.1374809294939041</v>
+        <v>-0.1239296719431877</v>
       </c>
     </row>
     <row r="48" spans="1:17">
       <c r="A48">
-        <v>0.2445306330919266</v>
+        <v>0.2396796494722366</v>
       </c>
       <c r="B48">
-        <v>0.2107041329145432</v>
+        <v>0.2176637053489685</v>
       </c>
       <c r="C48">
-        <v>0.4683302044868469</v>
+        <v>0.465215265750885</v>
       </c>
       <c r="D48">
-        <v>-0.2586875557899475</v>
+        <v>-0.2627837955951691</v>
       </c>
       <c r="E48">
-        <v>-0.01245014928281307</v>
+        <v>-0.01418656297028065</v>
       </c>
       <c r="F48">
-        <v>0.1886773854494095</v>
+        <v>0.1860650181770325</v>
       </c>
       <c r="G48">
-        <v>8.481306963403767E-07</v>
+        <v>8.523979886376765E-07</v>
       </c>
       <c r="H48">
-        <v>0.007603913545608521</v>
+        <v>-6.166386015138414E-07</v>
       </c>
       <c r="I48">
         <v>7.999236828482026E-08</v>
       </c>
       <c r="J48">
-        <v>-0.09118754416704178</v>
+        <v>-0.09507197886705399</v>
       </c>
       <c r="K48">
-        <v>0.1044903621077538</v>
+        <v>0.1046624332666397</v>
       </c>
       <c r="L48">
         <v>-9.655797272856148E-10</v>
       </c>
       <c r="M48">
-        <v>0.4386396706104279</v>
+        <v>0.4311828911304474</v>
       </c>
       <c r="N48">
-        <v>-0.2885849177837372</v>
+        <v>-0.2916721105575562</v>
       </c>
       <c r="O48">
-        <v>-0.113082654774189</v>
+        <v>-0.1162548959255219</v>
       </c>
       <c r="Q48">
-        <v>0.01505070365965366</v>
+        <v>0.01658876985311508</v>
       </c>
     </row>
     <row r="49" spans="1:17">
       <c r="A49">
-        <v>-0.1511800587177277</v>
+        <v>-0.1622579842805862</v>
       </c>
       <c r="B49">
-        <v>-1.181136042305297E-07</v>
+        <v>-4.988606150391206E-08</v>
       </c>
       <c r="C49">
-        <v>-0.185525968670845</v>
+        <v>-0.1904085129499435</v>
       </c>
       <c r="D49">
-        <v>-0.03286861628293991</v>
+        <v>-0.04083628207445145</v>
       </c>
       <c r="E49">
-        <v>-0.005872344598174095</v>
+        <v>-0.001736907288432121</v>
       </c>
       <c r="F49">
-        <v>0.3326249420642853</v>
+        <v>0.3279638290405273</v>
       </c>
       <c r="G49">
-        <v>-0.01581787690520287</v>
+        <v>-0.01581781916320324</v>
       </c>
       <c r="H49">
-        <v>2.139152638847008E-05</v>
+        <v>2.771288052372256E-07</v>
       </c>
       <c r="I49">
         <v>0.04881750047206879</v>
       </c>
       <c r="J49">
-        <v>0.1830773651599884</v>
+        <v>0.1782799810171127</v>
       </c>
       <c r="K49">
-        <v>0.07453268766403198</v>
+        <v>0.06927835941314697</v>
       </c>
       <c r="L49">
         <v>6.190867134137079E-05</v>
       </c>
       <c r="M49">
-        <v>-0.08933265507221222</v>
+        <v>-0.111953966319561</v>
       </c>
       <c r="N49">
-        <v>-0.01334738545119762</v>
+        <v>-0.01568492315709591</v>
       </c>
       <c r="O49">
-        <v>0.2967642545700073</v>
+        <v>0.2950175404548645</v>
       </c>
       <c r="Q49">
-        <v>-0.07152320444583893</v>
+        <v>-0.0443214513361454</v>
       </c>
     </row>
     <row r="50" spans="1:17">
       <c r="A50">
-        <v>0.1581433117389679</v>
+        <v>0.1599185019731522</v>
       </c>
       <c r="B50">
-        <v>-0.02149536460638046</v>
+        <v>-0.02637472748756409</v>
       </c>
       <c r="C50">
-        <v>-0.04954629391431808</v>
+        <v>-0.05080396309494972</v>
       </c>
       <c r="D50">
-        <v>0.003538339398801327</v>
+        <v>0.002896253252401948</v>
       </c>
       <c r="E50">
-        <v>2.347318059037207E-06</v>
+        <v>1.600176119609387E-06</v>
       </c>
       <c r="F50">
-        <v>-0.1807541400194168</v>
+        <v>-0.1900849640369415</v>
       </c>
       <c r="G50">
-        <v>-0.02088215202093124</v>
+        <v>-0.02088910713791847</v>
       </c>
       <c r="H50">
-        <v>-6.346745794871822E-05</v>
+        <v>-1.537155071673624E-06</v>
       </c>
       <c r="I50">
         <v>4.782532148084329E-10</v>
       </c>
       <c r="J50">
-        <v>0.07925216853618622</v>
+        <v>0.08268974721431732</v>
       </c>
       <c r="K50">
-        <v>-0.04910707101225853</v>
+        <v>-0.05285041779279709</v>
       </c>
       <c r="L50">
         <v>6.264975382919147E-08</v>
       </c>
       <c r="M50">
-        <v>-0.1257932037115097</v>
+        <v>-0.1301457285881042</v>
       </c>
       <c r="N50">
-        <v>-0.1780485957860947</v>
+        <v>-0.1871180087327957</v>
       </c>
       <c r="O50">
-        <v>0.08046934753656387</v>
+        <v>0.09186387807130814</v>
       </c>
       <c r="Q50">
-        <v>0.01013224199414253</v>
+        <v>0.007370593957602978</v>
       </c>
     </row>
     <row r="51" spans="1:17">
       <c r="A51">
-        <v>-0.4056082665920258</v>
+        <v>-0.408794492483139</v>
       </c>
       <c r="B51">
-        <v>-0.008561010472476482</v>
+        <v>-0.01336040534079075</v>
       </c>
       <c r="C51">
-        <v>-0.3802303075790405</v>
+        <v>-0.3824864029884338</v>
       </c>
       <c r="D51">
-        <v>0.3708589673042297</v>
+        <v>0.368340402841568</v>
       </c>
       <c r="E51">
-        <v>-0.004032248165458441</v>
+        <v>-0.01140501629561186</v>
       </c>
       <c r="F51">
-        <v>0.1222075745463371</v>
+        <v>0.1223775595426559</v>
       </c>
       <c r="G51">
         <v>0.0002146661427104846</v>
       </c>
       <c r="H51">
-        <v>0.002734538866207004</v>
+        <v>5.165160521514167E-10</v>
       </c>
       <c r="I51">
         <v>0.1168106570839882</v>
       </c>
       <c r="J51">
-        <v>0.1459505558013916</v>
+        <v>0.1450602412223816</v>
       </c>
       <c r="K51">
-        <v>-0.187244787812233</v>
+        <v>-0.1976242065429688</v>
       </c>
       <c r="L51">
         <v>7.103749552422975E-20</v>
       </c>
       <c r="M51">
-        <v>0.002702448517084122</v>
+        <v>-0.0133525412529707</v>
       </c>
       <c r="N51">
-        <v>0.4098265767097473</v>
+        <v>0.4100785851478577</v>
       </c>
       <c r="O51">
-        <v>0.3820303082466125</v>
+        <v>0.3839129507541656</v>
       </c>
       <c r="Q51">
-        <v>0.06901614367961884</v>
+        <v>0.08134797960519791</v>
       </c>
     </row>
     <row r="52" spans="1:17">
       <c r="A52">
-        <v>0.3021014630794525</v>
+        <v>0.2998274862766266</v>
       </c>
       <c r="B52">
-        <v>0.07292920351028442</v>
+        <v>0.07660984992980957</v>
       </c>
       <c r="C52">
-        <v>0.4346327781677246</v>
+        <v>0.4352651238441467</v>
       </c>
       <c r="D52">
-        <v>-0.2676064670085907</v>
+        <v>-0.2677308022975922</v>
       </c>
       <c r="E52">
-        <v>-0.01198005024343729</v>
+        <v>-0.003521705977618694</v>
       </c>
       <c r="F52">
-        <v>-0.1025774776935577</v>
+        <v>-0.1014623194932938</v>
       </c>
       <c r="G52">
-        <v>-2.567764795458061E-06</v>
+        <v>-2.607946271382389E-06</v>
       </c>
       <c r="H52">
-        <v>-0.005180403124541044</v>
+        <v>-2.385493758083612E-07</v>
       </c>
       <c r="I52">
         <v>-0.05516742169857025</v>
       </c>
       <c r="J52">
-        <v>0.303097128868103</v>
+        <v>0.3036252856254578</v>
       </c>
       <c r="K52">
-        <v>0.07799429446458817</v>
+        <v>0.07599304616451263</v>
       </c>
       <c r="L52">
         <v>2.41745055973297E-07</v>
       </c>
       <c r="M52">
-        <v>0.01120521780103445</v>
+        <v>0.005578339565545321</v>
       </c>
       <c r="N52">
-        <v>-0.2015060186386108</v>
+        <v>-0.2010219097137451</v>
       </c>
       <c r="O52">
-        <v>0.07535379379987717</v>
+        <v>0.07262576371431351</v>
       </c>
       <c r="Q52">
-        <v>-0.001981409732252359</v>
+        <v>-0.005392871331423521</v>
       </c>
     </row>
     <row r="53" spans="1:17">
       <c r="A53">
-        <v>-0.155799612402916</v>
+        <v>-0.1535912603139877</v>
       </c>
       <c r="B53">
-        <v>0.2590490877628326</v>
+        <v>0.255707710981369</v>
       </c>
       <c r="C53">
-        <v>0.07227541506290436</v>
+        <v>0.07502497732639313</v>
       </c>
       <c r="D53">
-        <v>-0.06336271017789841</v>
+        <v>-0.06082483381032944</v>
       </c>
       <c r="E53">
-        <v>-0.009039942175149918</v>
+        <v>-0.01068016607314348</v>
       </c>
       <c r="F53">
-        <v>-0.1934247314929962</v>
+        <v>-0.1896026581525803</v>
       </c>
       <c r="G53">
-        <v>0.06553228944540024</v>
+        <v>0.06554411351680756</v>
       </c>
       <c r="H53">
-        <v>0.02485665306448936</v>
+        <v>9.272881698052515E-07</v>
       </c>
       <c r="I53">
         <v>-1.321401583709303E-07</v>
       </c>
       <c r="J53">
-        <v>0.2524596750736237</v>
+        <v>0.255717933177948</v>
       </c>
       <c r="K53">
-        <v>0.3109884262084961</v>
+        <v>0.3129144310951233</v>
       </c>
       <c r="L53">
         <v>0.0005826816777698696</v>
       </c>
       <c r="M53">
-        <v>-0.1514482498168945</v>
+        <v>-0.1749601513147354</v>
       </c>
       <c r="N53">
-        <v>-0.04424524307250977</v>
+        <v>-0.04127941280603409</v>
       </c>
       <c r="O53">
-        <v>0.236536517739296</v>
+        <v>0.2394916415214539</v>
       </c>
       <c r="Q53">
-        <v>0.2985902726650238</v>
+        <v>0.2858589291572571</v>
       </c>
     </row>
     <row r="54" spans="1:17">
       <c r="A54">
-        <v>-0.02523194439709187</v>
+        <v>-0.02180639654397964</v>
       </c>
       <c r="B54">
-        <v>0.09978058934211731</v>
+        <v>0.1097455471754074</v>
       </c>
       <c r="C54">
-        <v>0.2871801555156708</v>
+        <v>0.2928610146045685</v>
       </c>
       <c r="D54">
-        <v>0.05061123892664909</v>
+        <v>0.05549240112304688</v>
       </c>
       <c r="E54">
-        <v>0.001418419182300568</v>
+        <v>0.002134301699697971</v>
       </c>
       <c r="F54">
-        <v>0.3826444745063782</v>
+        <v>0.3878342509269714</v>
       </c>
       <c r="G54">
-        <v>0.03799038380384445</v>
+        <v>0.03799973428249359</v>
       </c>
       <c r="H54">
-        <v>0.0001958149805432186</v>
+        <v>-7.872202445469156E-08</v>
       </c>
       <c r="I54">
         <v>-0.02743068896234035</v>
       </c>
       <c r="J54">
-        <v>0.02382905781269073</v>
+        <v>0.03032586164772511</v>
       </c>
       <c r="K54">
-        <v>-0.3566353023052216</v>
+        <v>-0.3521738350391388</v>
       </c>
       <c r="L54">
         <v>-9.422206517228915E-07</v>
       </c>
       <c r="M54">
-        <v>0.3836376965045929</v>
+        <v>0.3828519582748413</v>
       </c>
       <c r="N54">
-        <v>-0.4511966705322266</v>
+        <v>-0.4465733766555786</v>
       </c>
       <c r="O54">
-        <v>0.4122436940670013</v>
+        <v>0.422176331281662</v>
       </c>
       <c r="Q54">
-        <v>0.02915268950164318</v>
+        <v>0.02173438295722008</v>
       </c>
     </row>
     <row r="57" spans="1:17">
       <c r="A57">
-        <v>-0.004987639840692282</v>
+        <v>-0.007569501642137766</v>
       </c>
       <c r="B57">
-        <v>-0.00406472384929657</v>
+        <v>-0.05227402597665787</v>
       </c>
       <c r="C57">
-        <v>-2.028886683547171E-06</v>
+        <v>0.02217996679246426</v>
       </c>
       <c r="D57">
-        <v>0.005767886526882648</v>
+        <v>0.06567803770303726</v>
       </c>
       <c r="E57">
-        <v>-0.005546287167817354</v>
+        <v>0.003785547567531466</v>
       </c>
       <c r="F57">
-        <v>-0.006522941868752241</v>
+        <v>0.002932505449280143</v>
       </c>
       <c r="G57">
-        <v>7.840125379257228E-19</v>
+        <v>0.009830920957028866</v>
       </c>
       <c r="H57">
-        <v>8.27784460852854E-05</v>
+        <v>-7.725209798081778E-06</v>
       </c>
       <c r="I57">
-        <v>-0.01670173555612564</v>
+        <v>-0.03156908601522446</v>
       </c>
       <c r="J57">
-        <v>-4.116042691748589E-05</v>
+        <v>-0.03535209596157074</v>
       </c>
       <c r="K57">
-        <v>9.14047859623679E-07</v>
+        <v>0.04967555403709412</v>
       </c>
       <c r="L57">
-        <v>1.893382795969956E-05</v>
+        <v>-0.04226420819759369</v>
       </c>
       <c r="M57">
-        <v>0.01720618642866611</v>
+        <v>0.07009644061326981</v>
       </c>
       <c r="N57">
-        <v>1.451304115107632E-06</v>
+        <v>0.03037702664732933</v>
       </c>
       <c r="O57">
-        <v>-1.83645333891036E-05</v>
+        <v>-0.001445501111447811</v>
       </c>
       <c r="Q57">
-        <v>-0.01987113617360592</v>
+        <v>-0.04748798906803131</v>
       </c>
     </row>
     <row r="58" spans="1:17">
       <c r="A58">
-        <v>0.2275195270776749</v>
+        <v>0.2204605787992477</v>
       </c>
       <c r="B58">
-        <v>-0.3771900832653046</v>
+        <v>-0.3697133958339691</v>
       </c>
       <c r="C58">
-        <v>-0.00159810297191143</v>
+        <v>0.005436311475932598</v>
       </c>
       <c r="D58">
-        <v>0.1947411149740219</v>
+        <v>0.1834677904844284</v>
       </c>
       <c r="E58">
-        <v>0.05304499343037605</v>
+        <v>0.0497557632625103</v>
       </c>
       <c r="F58">
-        <v>0.1631438434123993</v>
+        <v>0.1589208841323853</v>
       </c>
       <c r="G58">
-        <v>-0.01455661840736866</v>
+        <v>-0.01476471684873104</v>
       </c>
       <c r="H58">
-        <v>0.2250128537416458</v>
+        <v>0.2236419022083282</v>
       </c>
       <c r="I58">
-        <v>-0.3024962246417999</v>
+        <v>-0.3055022358894348</v>
       </c>
       <c r="J58">
-        <v>-0.0748516246676445</v>
+        <v>-0.07649333029985428</v>
       </c>
       <c r="K58">
-        <v>0.03427555039525032</v>
+        <v>0.02641934156417847</v>
       </c>
       <c r="L58">
-        <v>0.1886956989765167</v>
+        <v>0.1891452372074127</v>
       </c>
       <c r="M58">
-        <v>0.1471867710351944</v>
+        <v>0.1444837749004364</v>
       </c>
       <c r="N58">
-        <v>0.1362967491149902</v>
+        <v>0.1336303502321243</v>
       </c>
       <c r="O58">
-        <v>0.07044260948896408</v>
+        <v>0.06753129512071609</v>
       </c>
       <c r="Q58">
-        <v>-0.104475349187851</v>
+        <v>-0.1192265152931213</v>
       </c>
     </row>
     <row r="59" spans="1:17">
       <c r="A59">
-        <v>-0.1664841026067734</v>
+        <v>-0.1635665893554688</v>
       </c>
       <c r="B59">
-        <v>0.3677668869495392</v>
+        <v>0.3614034056663513</v>
       </c>
       <c r="C59">
-        <v>-0.03523388504981995</v>
+        <v>-0.03208195045590401</v>
       </c>
       <c r="D59">
-        <v>-0.1107313856482506</v>
+        <v>-0.1060510873794556</v>
       </c>
       <c r="E59">
-        <v>-0.2635255753993988</v>
+        <v>-0.2655212581157684</v>
       </c>
       <c r="F59">
-        <v>-0.00179708341602236</v>
+        <v>-0.00550880329683423</v>
       </c>
       <c r="G59">
-        <v>-0.002234259154647589</v>
+        <v>-0.004209186881780624</v>
       </c>
       <c r="H59">
-        <v>0.008359871804714203</v>
+        <v>0.01055710203945637</v>
       </c>
       <c r="I59">
-        <v>0.1269473433494568</v>
+        <v>0.1244605109095573</v>
       </c>
       <c r="J59">
-        <v>-0.01600618101656437</v>
+        <v>-0.01145322900265455</v>
       </c>
       <c r="K59">
-        <v>-0.04158805683255196</v>
+        <v>-0.03370918333530426</v>
       </c>
       <c r="L59">
-        <v>-0.347597599029541</v>
+        <v>-0.3526649475097656</v>
       </c>
       <c r="M59">
-        <v>0.3815108835697174</v>
+        <v>0.3808871805667877</v>
       </c>
       <c r="N59">
-        <v>-0.412246972322464</v>
+        <v>-0.4160151481628418</v>
       </c>
       <c r="O59">
-        <v>0.3646811544895172</v>
+        <v>0.3658458292484283</v>
       </c>
       <c r="Q59">
-        <v>-0.04946991801261902</v>
+        <v>-0.05418453365564346</v>
       </c>
     </row>
     <row r="60" spans="1:17">
       <c r="A60">
-        <v>-0.001734001911245286</v>
+        <v>-0.0002089879853883758</v>
       </c>
       <c r="B60">
-        <v>-0.00534835085272789</v>
+        <v>-2.038991938137088E-18</v>
       </c>
       <c r="C60">
-        <v>0.0001225924352183938</v>
+        <v>-1.215083102579229E-06</v>
       </c>
       <c r="D60">
-        <v>-0.003447976661846042</v>
+        <v>-9.799924737308174E-05</v>
       </c>
       <c r="E60">
-        <v>-0.007299335673451424</v>
+        <v>-0.002252800390124321</v>
       </c>
       <c r="F60">
-        <v>-0.004832423757761717</v>
+        <v>-0.001445704256184399</v>
       </c>
       <c r="G60">
         <v>-8.525697694494738E-07</v>
       </c>
       <c r="H60">
-        <v>-0.004844045732170343</v>
+        <v>-8.61063672346063E-05</v>
       </c>
       <c r="I60">
-        <v>-0.004957661498337984</v>
+        <v>-0.001476107281632721</v>
       </c>
       <c r="J60">
-        <v>-0.004672426730394363</v>
+        <v>-7.757988029766238E-09</v>
       </c>
       <c r="K60">
-        <v>5.389247235143557E-07</v>
+        <v>1.293499565235834E-07</v>
       </c>
       <c r="L60">
-        <v>-0.00350974197499454</v>
+        <v>3.873261888998059E-08</v>
       </c>
       <c r="M60">
-        <v>-0.004908580332994461</v>
+        <v>-0.001265577273443341</v>
       </c>
       <c r="N60">
-        <v>6.569797733391169E-06</v>
+        <v>4.837354481423972E-07</v>
       </c>
       <c r="O60">
-        <v>-0.004873318132013083</v>
+        <v>4.239095687808003E-06</v>
       </c>
       <c r="Q60">
-        <v>-0.005150087177753448</v>
+        <v>-0.005615600384771824</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -2303,7 +2303,7 @@
         <v>-5.317658064996067E-07</v>
       </c>
       <c r="B61">
-        <v>-0.01298469956964254</v>
+        <v>0.001948701217770576</v>
       </c>
       <c r="C61">
         <v>-0.2058815658092499</v>
@@ -2312,340 +2312,340 @@
         <v>-0.002947651082649827</v>
       </c>
       <c r="E61">
-        <v>0.09076494723558426</v>
+        <v>0.1480000168085098</v>
       </c>
       <c r="F61">
-        <v>-0.06760977953672409</v>
+        <v>-0.1143595278263092</v>
       </c>
       <c r="G61">
         <v>0.1721467822790146</v>
       </c>
       <c r="H61">
-        <v>-0.005226798821240664</v>
+        <v>-0.01122566498816013</v>
       </c>
       <c r="I61">
-        <v>-0.007767705712467432</v>
+        <v>0.01244648080319166</v>
       </c>
       <c r="J61">
-        <v>-0.0109509751200676</v>
+        <v>-0.01660990715026855</v>
       </c>
       <c r="K61">
         <v>-3.081167676555197E-07</v>
       </c>
       <c r="L61">
-        <v>-0.01919602230191231</v>
+        <v>-0.02083286270499229</v>
       </c>
       <c r="M61">
-        <v>-0.08395911753177643</v>
+        <v>-0.1134535595774651</v>
       </c>
       <c r="N61">
-        <v>-0.001087108859792352</v>
+        <v>3.611477694676068E-08</v>
       </c>
       <c r="O61">
-        <v>-0.02422123588621616</v>
+        <v>-0.03916024789214134</v>
       </c>
       <c r="Q61">
-        <v>-0.06476548314094543</v>
+        <v>-0.06202749162912369</v>
       </c>
     </row>
     <row r="62" spans="1:17">
       <c r="A62">
-        <v>-0.4198038280010223</v>
+        <v>-0.4242255985736847</v>
       </c>
       <c r="B62">
-        <v>-0.3358325064182281</v>
+        <v>-0.3370487093925476</v>
       </c>
       <c r="C62">
-        <v>0.0767403170466423</v>
+        <v>0.06968457996845245</v>
       </c>
       <c r="D62">
-        <v>-0.005283007863909006</v>
+        <v>-0.01333011500537395</v>
       </c>
       <c r="E62">
-        <v>-0.2697775661945343</v>
+        <v>-0.2736946940422058</v>
       </c>
       <c r="F62">
-        <v>0.3959852755069733</v>
+        <v>0.3926222622394562</v>
       </c>
       <c r="G62">
-        <v>0.1234204173088074</v>
+        <v>0.1236657500267029</v>
       </c>
       <c r="H62">
-        <v>0.3573806881904602</v>
+        <v>0.3475930690765381</v>
       </c>
       <c r="I62">
-        <v>0.3172584772109985</v>
+        <v>0.3099546134471893</v>
       </c>
       <c r="J62">
-        <v>0.3928178250789642</v>
+        <v>0.3861629962921143</v>
       </c>
       <c r="K62">
-        <v>0.04628767445683479</v>
+        <v>0.03890351578593254</v>
       </c>
       <c r="L62">
-        <v>0.3288109302520752</v>
+        <v>0.3333691954612732</v>
       </c>
       <c r="M62">
-        <v>0.1965972930192947</v>
+        <v>0.1916812360286713</v>
       </c>
       <c r="N62">
-        <v>0.3531248569488525</v>
+        <v>0.362524151802063</v>
       </c>
       <c r="O62">
-        <v>-0.4299743175506592</v>
+        <v>-0.4382191598415375</v>
       </c>
       <c r="Q62">
-        <v>-0.1421887129545212</v>
+        <v>-0.1400502324104309</v>
       </c>
     </row>
     <row r="63" spans="1:17">
       <c r="A63">
-        <v>0.1320456564426422</v>
+        <v>0.1526151150465012</v>
       </c>
       <c r="B63">
-        <v>0.2633671462535858</v>
+        <v>0.2723596394062042</v>
       </c>
       <c r="C63">
-        <v>-0.003536404110491276</v>
+        <v>-0.004830463323742151</v>
       </c>
       <c r="D63">
-        <v>-0.1856012493371964</v>
+        <v>-0.1749162673950195</v>
       </c>
       <c r="E63">
-        <v>-0.2039248943328857</v>
+        <v>-0.1993478983640671</v>
       </c>
       <c r="F63">
-        <v>0.2731313705444336</v>
+        <v>0.2747678458690643</v>
       </c>
       <c r="G63">
-        <v>0.0002481247938703746</v>
+        <v>-0.0002596825652290136</v>
       </c>
       <c r="H63">
-        <v>-0.02512749284505844</v>
+        <v>-0.02028006501495838</v>
       </c>
       <c r="I63">
-        <v>0.2847785949707031</v>
+        <v>0.2883553206920624</v>
       </c>
       <c r="J63">
-        <v>-0.1934238821268082</v>
+        <v>-0.188057541847229</v>
       </c>
       <c r="K63">
-        <v>0.006930865347385406</v>
+        <v>0.001977854873985052</v>
       </c>
       <c r="L63">
-        <v>0.01499159634113312</v>
+        <v>0.02642822265625</v>
       </c>
       <c r="M63">
-        <v>0.2847772538661957</v>
+        <v>0.2897493839263916</v>
       </c>
       <c r="N63">
-        <v>0.1942756921052933</v>
+        <v>0.1925545036792755</v>
       </c>
       <c r="O63">
-        <v>-0.4557773470878601</v>
+        <v>-0.4538152515888214</v>
       </c>
       <c r="Q63">
-        <v>-0.245493158698082</v>
+        <v>-0.2398160099983215</v>
       </c>
     </row>
     <row r="64" spans="1:17">
       <c r="A64">
-        <v>0.253322035074234</v>
+        <v>0.2592049837112427</v>
       </c>
       <c r="B64">
-        <v>-0.2980717718601227</v>
+        <v>-0.2957746684551239</v>
       </c>
       <c r="C64">
-        <v>-0.04213385283946991</v>
+        <v>-0.03062828816473484</v>
       </c>
       <c r="D64">
-        <v>-0.02801037207245827</v>
+        <v>-0.02014845982193947</v>
       </c>
       <c r="E64">
-        <v>-0.2432406544685364</v>
+        <v>-0.2441718876361847</v>
       </c>
       <c r="F64">
-        <v>0.3168142735958099</v>
+        <v>0.3172717094421387</v>
       </c>
       <c r="G64">
-        <v>0.1906461715698242</v>
+        <v>0.1906332224607468</v>
       </c>
       <c r="H64">
-        <v>-0.1014181151986122</v>
+        <v>-0.1040105298161507</v>
       </c>
       <c r="I64">
-        <v>0.4332052171230316</v>
+        <v>0.4320534765720367</v>
       </c>
       <c r="J64">
-        <v>-0.01953363232314587</v>
+        <v>-0.0005305677186697721</v>
       </c>
       <c r="K64">
-        <v>-0.01424470171332359</v>
+        <v>-0.01264088228344917</v>
       </c>
       <c r="L64">
         <v>0.2154740244150162</v>
       </c>
       <c r="M64">
-        <v>-0.4222503006458282</v>
+        <v>-0.4236893057823181</v>
       </c>
       <c r="N64">
-        <v>-0.08641898632049561</v>
+        <v>-0.1042615696787834</v>
       </c>
       <c r="O64">
-        <v>0.2061730325222015</v>
+        <v>0.2077972292900085</v>
       </c>
       <c r="Q64">
-        <v>0.006632989272475243</v>
+        <v>0.02215107902884483</v>
       </c>
     </row>
     <row r="65" spans="1:17">
       <c r="A65">
-        <v>0.1454208791255951</v>
+        <v>0.1454567313194275</v>
       </c>
       <c r="B65">
-        <v>0.08522666990756989</v>
+        <v>0.07154924422502518</v>
       </c>
       <c r="C65">
-        <v>-0.06424663215875626</v>
+        <v>-0.06422766298055649</v>
       </c>
       <c r="D65">
-        <v>-2.6382697342342E-06</v>
+        <v>-2.649762109285803E-06</v>
       </c>
       <c r="E65">
-        <v>-0.4442151486873627</v>
+        <v>-0.4477815926074982</v>
       </c>
       <c r="F65">
-        <v>0.03891327604651451</v>
+        <v>0.02327590249478817</v>
       </c>
       <c r="G65">
-        <v>3.227375486858364E-07</v>
+        <v>3.39218331646407E-07</v>
       </c>
       <c r="H65">
-        <v>0.2394923269748688</v>
+        <v>0.2213108241558075</v>
       </c>
       <c r="I65">
-        <v>-0.3316235542297363</v>
+        <v>-0.3308868110179901</v>
       </c>
       <c r="J65">
-        <v>-0.3577196300029755</v>
+        <v>-0.3585657477378845</v>
       </c>
       <c r="K65">
-        <v>-2.675073801583494E-06</v>
+        <v>-2.677924385352526E-06</v>
       </c>
       <c r="L65">
-        <v>0.2384263128042221</v>
+        <v>0.220358744263649</v>
       </c>
       <c r="M65">
-        <v>0.1645322293043137</v>
+        <v>0.1489215344190598</v>
       </c>
       <c r="N65">
-        <v>2.324961769772926E-07</v>
+        <v>1.196428485172873E-07</v>
       </c>
       <c r="O65">
-        <v>0.3160206079483032</v>
+        <v>0.2965687215328217</v>
       </c>
       <c r="Q65">
-        <v>-0.03230460733175278</v>
+        <v>-0.04211097955703735</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66">
-        <v>-0.2417312115430832</v>
+        <v>-0.2415283620357513</v>
       </c>
       <c r="B66">
-        <v>-0.1114616766571999</v>
+        <v>-0.1114331111311913</v>
       </c>
       <c r="C66">
-        <v>0.2396713197231293</v>
+        <v>0.2396786212921143</v>
       </c>
       <c r="D66">
-        <v>0.1780940741300583</v>
+        <v>0.1784435212612152</v>
       </c>
       <c r="E66">
-        <v>0.170369952917099</v>
+        <v>0.1774851828813553</v>
       </c>
       <c r="F66">
-        <v>4.778437141794711E-05</v>
+        <v>-0.003570939647033811</v>
       </c>
       <c r="G66">
-        <v>-0.1802997291088104</v>
+        <v>-0.1802988201379776</v>
       </c>
       <c r="H66">
-        <v>0.2006234526634216</v>
+        <v>0.2013015747070312</v>
       </c>
       <c r="I66">
-        <v>-0.002039466286078095</v>
+        <v>-0.01214530505239964</v>
       </c>
       <c r="J66">
-        <v>3.953679481583094E-07</v>
+        <v>3.952183362798678E-07</v>
       </c>
       <c r="K66">
-        <v>-9.94407764665084E-06</v>
+        <v>-2.353717754033369E-08</v>
       </c>
       <c r="L66">
-        <v>-0.001701413188129663</v>
+        <v>-0.001700759865343571</v>
       </c>
       <c r="M66">
-        <v>-0.2753956615924835</v>
+        <v>-0.2766487598419189</v>
       </c>
       <c r="N66">
-        <v>0.09719480574131012</v>
+        <v>0.09722127020359039</v>
       </c>
       <c r="O66">
-        <v>-2.86623230749683E-06</v>
+        <v>-0.0006450007786042988</v>
       </c>
       <c r="Q66">
-        <v>-0.08980029821395874</v>
+        <v>-0.09189531952142715</v>
       </c>
     </row>
     <row r="67" spans="1:17">
       <c r="A67">
-        <v>-0.05205364897847176</v>
+        <v>-0.07135467976331711</v>
       </c>
       <c r="B67">
-        <v>-0.01126890536397696</v>
+        <v>-0.007843847386538982</v>
       </c>
       <c r="C67">
-        <v>-0.1627397239208221</v>
+        <v>-0.1597139835357666</v>
       </c>
       <c r="D67">
-        <v>0.2619676291942596</v>
+        <v>0.2402385771274567</v>
       </c>
       <c r="E67">
-        <v>0.3380360901355743</v>
+        <v>0.3407940566539764</v>
       </c>
       <c r="F67">
-        <v>-0.1076530441641808</v>
+        <v>-0.114873930811882</v>
       </c>
       <c r="G67">
-        <v>0.04785345122218132</v>
+        <v>0.04631825163960457</v>
       </c>
       <c r="H67">
-        <v>0.06269782036542892</v>
+        <v>0.06392066925764084</v>
       </c>
       <c r="I67">
-        <v>0.2179436832666397</v>
+        <v>0.2160491645336151</v>
       </c>
       <c r="J67">
-        <v>-0.07257189601659775</v>
+        <v>-0.06509067863225937</v>
       </c>
       <c r="K67">
-        <v>0.01478699315339327</v>
+        <v>0.01156479865312576</v>
       </c>
       <c r="L67">
-        <v>0.392847865819931</v>
+        <v>0.4040400087833405</v>
       </c>
       <c r="M67">
-        <v>0.1180150061845779</v>
+        <v>0.1184200048446655</v>
       </c>
       <c r="N67">
-        <v>0.1579026728868484</v>
+        <v>0.1418487280607224</v>
       </c>
       <c r="O67">
-        <v>-0.03260598704218864</v>
+        <v>-0.02988419309258461</v>
       </c>
       <c r="Q67">
-        <v>0.1632344275712967</v>
+        <v>0.1606055349111557</v>
       </c>
     </row>
     <row r="68" spans="1:17">
@@ -2653,7 +2653,7 @@
         <v>0.03426491096615791</v>
       </c>
       <c r="B68">
-        <v>0.1747256219387054</v>
+        <v>0.174928218126297</v>
       </c>
       <c r="C68">
         <v>0.1356670707464218</v>
@@ -2662,40 +2662,40 @@
         <v>0.09152939170598984</v>
       </c>
       <c r="E68">
-        <v>0.06912150233983994</v>
+        <v>0.07037993520498276</v>
       </c>
       <c r="F68">
-        <v>0.178612694144249</v>
+        <v>0.1782323271036148</v>
       </c>
       <c r="G68">
         <v>-0.06598754227161407</v>
       </c>
       <c r="H68">
-        <v>-0.08349422365427017</v>
+        <v>-0.07845300436019897</v>
       </c>
       <c r="I68">
-        <v>-0.2844651341438293</v>
+        <v>-0.2809379398822784</v>
       </c>
       <c r="J68">
-        <v>0.3329493999481201</v>
+        <v>0.3366671800613403</v>
       </c>
       <c r="K68">
         <v>-0.0004328940121922642</v>
       </c>
       <c r="L68">
-        <v>0.002663982333615422</v>
+        <v>0.004730762913823128</v>
       </c>
       <c r="M68">
-        <v>-0.285638153553009</v>
+        <v>-0.2848731279373169</v>
       </c>
       <c r="N68">
-        <v>-0.1693524867296219</v>
+        <v>-0.1764285415410995</v>
       </c>
       <c r="O68">
-        <v>-0.06821074336767197</v>
+        <v>-0.05910775065422058</v>
       </c>
       <c r="Q68">
-        <v>-0.1154214814305305</v>
+        <v>-0.1072707399725914</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -2750,652 +2750,652 @@
     </row>
     <row r="70" spans="1:17">
       <c r="A70">
-        <v>0.05856166034936905</v>
+        <v>0.0555078536272049</v>
       </c>
       <c r="B70">
-        <v>-0.2288554906845093</v>
+        <v>-0.2292813956737518</v>
       </c>
       <c r="C70">
-        <v>-0.06930603832006454</v>
+        <v>-0.06352382153272629</v>
       </c>
       <c r="D70">
-        <v>0.05022232979536057</v>
+        <v>0.0555431954562664</v>
       </c>
       <c r="E70">
-        <v>0.07206820696592331</v>
+        <v>0.07121258229017258</v>
       </c>
       <c r="F70">
-        <v>0.1197926476597786</v>
+        <v>0.1189847216010094</v>
       </c>
       <c r="G70">
-        <v>-0.1430869251489639</v>
+        <v>-0.1447033882141113</v>
       </c>
       <c r="H70">
-        <v>0.1668838709592819</v>
+        <v>0.1665944010019302</v>
       </c>
       <c r="I70">
-        <v>0.4176476001739502</v>
+        <v>0.4163958728313446</v>
       </c>
       <c r="J70">
-        <v>-0.3030471205711365</v>
+        <v>-0.3126799166202545</v>
       </c>
       <c r="K70">
-        <v>0.006748705171048641</v>
+        <v>0.002666051965206861</v>
       </c>
       <c r="L70">
-        <v>-0.3504334986209869</v>
+        <v>-0.3562342524528503</v>
       </c>
       <c r="M70">
-        <v>-0.01489784102886915</v>
+        <v>-0.01646754890680313</v>
       </c>
       <c r="N70">
-        <v>0.2234143316745758</v>
+        <v>0.2281143665313721</v>
       </c>
       <c r="O70">
-        <v>0.3502953946590424</v>
+        <v>0.3514710068702698</v>
       </c>
       <c r="Q70">
-        <v>-0.001148577313870192</v>
+        <v>-0.004458490759134293</v>
       </c>
     </row>
     <row r="71" spans="1:17">
       <c r="A71">
-        <v>-0.0138269541785121</v>
+        <v>-0.009648198261857033</v>
       </c>
       <c r="B71">
-        <v>0.23370660841465</v>
+        <v>0.2269544154405594</v>
       </c>
       <c r="C71">
-        <v>0.3039248585700989</v>
+        <v>0.2730908691883087</v>
       </c>
       <c r="D71">
-        <v>-0.153759777545929</v>
+        <v>-0.1569087207317352</v>
       </c>
       <c r="E71">
-        <v>-0.2097492665052414</v>
+        <v>-0.207925409078598</v>
       </c>
       <c r="F71">
-        <v>0.374749630689621</v>
+        <v>0.3806228041648865</v>
       </c>
       <c r="G71">
-        <v>-0.1779023855924606</v>
+        <v>-0.1743590384721756</v>
       </c>
       <c r="H71">
-        <v>0.1768929362297058</v>
+        <v>0.1715212464332581</v>
       </c>
       <c r="I71">
-        <v>-0.02772773988544941</v>
+        <v>-0.02565942890942097</v>
       </c>
       <c r="J71">
-        <v>-0.2768742442131042</v>
+        <v>-0.2878896296024323</v>
       </c>
       <c r="K71">
-        <v>0.07498269528150558</v>
+        <v>0.06738973408937454</v>
       </c>
       <c r="L71">
-        <v>-0.3017571866512299</v>
+        <v>-0.3052732646465302</v>
       </c>
       <c r="M71">
-        <v>-0.02948739379644394</v>
+        <v>-0.02885118313133717</v>
       </c>
       <c r="N71">
-        <v>0.09506958723068237</v>
+        <v>0.08173947036266327</v>
       </c>
       <c r="O71">
-        <v>0.08324305713176727</v>
+        <v>0.0820208266377449</v>
       </c>
       <c r="Q71">
-        <v>-0.1243916153907776</v>
+        <v>-0.1217965260148048</v>
       </c>
     </row>
     <row r="74" spans="1:17">
       <c r="A74">
-        <v>0.1955542415380478</v>
+        <v>0.1011974066495895</v>
       </c>
       <c r="B74">
-        <v>0.244455561041832</v>
+        <v>0.2238318622112274</v>
       </c>
       <c r="C74">
-        <v>-0.148880809545517</v>
+        <v>-0.1628094166517258</v>
       </c>
       <c r="D74">
-        <v>-0.4492203295230865</v>
+        <v>-0.448513001203537</v>
       </c>
       <c r="E74">
-        <v>-0.4055952131748199</v>
+        <v>-0.3995700478553772</v>
       </c>
       <c r="F74">
-        <v>-0.3108130395412445</v>
+        <v>-0.3288167715072632</v>
       </c>
       <c r="G74">
-        <v>-0.4481717050075531</v>
+        <v>-0.4329995810985565</v>
       </c>
       <c r="H74">
-        <v>0.03358727321028709</v>
+        <v>0.002426996827125549</v>
       </c>
       <c r="I74">
-        <v>0.08623462170362473</v>
+        <v>0.08618208765983582</v>
       </c>
       <c r="J74">
-        <v>0.002954953815788031</v>
+        <v>0.004130177665501833</v>
       </c>
       <c r="K74">
-        <v>0.4319316744804382</v>
+        <v>0.4212759733200073</v>
       </c>
       <c r="L74">
-        <v>0.002299546962603927</v>
+        <v>0.02727633155882359</v>
       </c>
       <c r="M74">
         <v>-0.1871657520532608</v>
       </c>
       <c r="N74">
-        <v>-0.3764066100120544</v>
+        <v>-0.369462639093399</v>
       </c>
       <c r="O74">
-        <v>0.1574117094278336</v>
+        <v>0.1415285021066666</v>
       </c>
       <c r="Q74">
-        <v>0.2728680372238159</v>
+        <v>0.2721457183361053</v>
       </c>
     </row>
     <row r="75" spans="1:17">
       <c r="A75">
-        <v>-0.2596646845340729</v>
+        <v>-0.2724531590938568</v>
       </c>
       <c r="B75">
-        <v>-0.3333405256271362</v>
+        <v>-0.343404620885849</v>
       </c>
       <c r="C75">
-        <v>-0.3271262645721436</v>
+        <v>-0.3229948878288269</v>
       </c>
       <c r="D75">
-        <v>-0.3489544689655304</v>
+        <v>-0.3474057614803314</v>
       </c>
       <c r="E75">
-        <v>0.2389866560697556</v>
+        <v>0.2401676177978516</v>
       </c>
       <c r="F75">
-        <v>0.3227335512638092</v>
+        <v>0.3203555941581726</v>
       </c>
       <c r="G75">
-        <v>0.477502316236496</v>
+        <v>0.4801400601863861</v>
       </c>
       <c r="H75">
-        <v>-0.357251763343811</v>
+        <v>-0.351962685585022</v>
       </c>
       <c r="I75">
-        <v>-0.2293453365564346</v>
+        <v>-0.2309398651123047</v>
       </c>
       <c r="J75">
-        <v>0.09435936808586121</v>
+        <v>0.1052279993891716</v>
       </c>
       <c r="K75">
-        <v>0.06034426391124725</v>
+        <v>0.0656154528260231</v>
       </c>
       <c r="L75">
-        <v>-0.4529072344303131</v>
+        <v>-0.438918799161911</v>
       </c>
       <c r="M75">
         <v>-0.2854933142662048</v>
       </c>
       <c r="N75">
-        <v>-0.3121688365936279</v>
+        <v>-0.3094950914382935</v>
       </c>
       <c r="O75">
-        <v>0.1968614310026169</v>
+        <v>0.1977957189083099</v>
       </c>
       <c r="Q75">
-        <v>-0.05822067335247993</v>
+        <v>-0.05742783099412918</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="A76">
-        <v>0.4247061312198639</v>
+        <v>0.4248446524143219</v>
       </c>
       <c r="B76">
-        <v>0.4719003438949585</v>
+        <v>0.4675652384757996</v>
       </c>
       <c r="C76">
-        <v>-0.4450461268424988</v>
+        <v>-0.4420274794101715</v>
       </c>
       <c r="D76">
-        <v>0.1063891425728798</v>
+        <v>0.1083678528666496</v>
       </c>
       <c r="E76">
-        <v>0.3122852146625519</v>
+        <v>0.3038278222084045</v>
       </c>
       <c r="F76">
-        <v>0.4229176938533783</v>
+        <v>0.4208153486251831</v>
       </c>
       <c r="G76">
-        <v>-0.03320113942027092</v>
+        <v>-0.03318754956126213</v>
       </c>
       <c r="H76">
-        <v>-0.08541475981473923</v>
+        <v>-0.09061456471681595</v>
       </c>
       <c r="I76">
-        <v>-0.450224757194519</v>
+        <v>-0.4515248537063599</v>
       </c>
       <c r="J76">
-        <v>-0.3229638636112213</v>
+        <v>-0.3405115008354187</v>
       </c>
       <c r="K76">
-        <v>0.06233405321836472</v>
+        <v>0.06431169062852859</v>
       </c>
       <c r="L76">
-        <v>-0.02832691371440887</v>
+        <v>-0.02325132302939892</v>
       </c>
       <c r="M76">
         <v>-0.2625187337398529</v>
       </c>
       <c r="N76">
-        <v>0.2654933333396912</v>
+        <v>0.2674592733383179</v>
       </c>
       <c r="O76">
-        <v>0.2012870311737061</v>
+        <v>0.1997740864753723</v>
       </c>
       <c r="Q76">
-        <v>-0.1867632269859314</v>
+        <v>-0.1840610951185226</v>
       </c>
     </row>
     <row r="77" spans="1:17">
       <c r="A77">
-        <v>0.04277124628424644</v>
+        <v>-0.01037456188350916</v>
       </c>
       <c r="B77">
-        <v>-0.2241380214691162</v>
+        <v>-0.2351546436548233</v>
       </c>
       <c r="C77">
-        <v>-0.2335635870695114</v>
+        <v>-0.2309645414352417</v>
       </c>
       <c r="D77">
-        <v>0.1258926540613174</v>
+        <v>0.1262752115726471</v>
       </c>
       <c r="E77">
-        <v>-0.2649059891700745</v>
+        <v>-0.280325710773468</v>
       </c>
       <c r="F77">
-        <v>-0.3401774764060974</v>
+        <v>-0.3339777588844299</v>
       </c>
       <c r="G77">
-        <v>0.4385212361812592</v>
+        <v>0.4389635324478149</v>
       </c>
       <c r="H77">
-        <v>-0.4314252436161041</v>
+        <v>-0.43846395611763</v>
       </c>
       <c r="I77">
-        <v>-0.2505591809749603</v>
+        <v>-0.2519882917404175</v>
       </c>
       <c r="J77">
-        <v>-0.3713774681091309</v>
+        <v>-0.3701381087303162</v>
       </c>
       <c r="K77">
-        <v>0.1154417023062706</v>
+        <v>0.1214122921228409</v>
       </c>
       <c r="L77">
-        <v>0.05842908471822739</v>
+        <v>0.05364537984132767</v>
       </c>
       <c r="M77">
         <v>-0.2426954209804535</v>
       </c>
       <c r="N77">
-        <v>-0.4746813774108887</v>
+        <v>-0.4840503334999084</v>
       </c>
       <c r="O77">
-        <v>0.06924934685230255</v>
+        <v>0.06266538053750992</v>
       </c>
       <c r="Q77">
-        <v>-0.2429996430873871</v>
+        <v>-0.2367291301488876</v>
       </c>
     </row>
     <row r="78" spans="1:17">
       <c r="A78">
-        <v>-0.2236060202121735</v>
+        <v>-0.2887874245643616</v>
       </c>
       <c r="B78">
-        <v>-0.489093154668808</v>
+        <v>-0.4964783489704132</v>
       </c>
       <c r="C78">
-        <v>0.1900715082883835</v>
+        <v>0.1926617175340652</v>
       </c>
       <c r="D78">
-        <v>-0.1020863428711891</v>
+        <v>-0.1013494729995728</v>
       </c>
       <c r="E78">
-        <v>0.0471324697136879</v>
+        <v>0.04366151615977287</v>
       </c>
       <c r="F78">
-        <v>0.1471705287694931</v>
+        <v>0.1606588065624237</v>
       </c>
       <c r="G78">
-        <v>0.3626827001571655</v>
+        <v>0.3523708283901215</v>
       </c>
       <c r="H78">
-        <v>0.3681247234344482</v>
+        <v>0.3650492131710052</v>
       </c>
       <c r="I78">
-        <v>-0.006262322887778282</v>
+        <v>3.515737262205221E-05</v>
       </c>
       <c r="J78">
-        <v>-0.3968794047832489</v>
+        <v>-0.3957715332508087</v>
       </c>
       <c r="K78">
-        <v>-0.07710874825716019</v>
+        <v>-0.07614593207836151</v>
       </c>
       <c r="L78">
-        <v>-0.3865165412425995</v>
+        <v>-0.3893004953861237</v>
       </c>
       <c r="M78">
         <v>0.1738163977861404</v>
       </c>
       <c r="N78">
-        <v>-0.6270038485527039</v>
+        <v>-0.6294139623641968</v>
       </c>
       <c r="O78">
-        <v>-0.5399398803710938</v>
+        <v>-0.5488042831420898</v>
       </c>
       <c r="Q78">
-        <v>0.1777685731649399</v>
+        <v>0.1751993894577026</v>
       </c>
     </row>
     <row r="79" spans="1:17">
       <c r="A79">
-        <v>-0.3597381114959717</v>
+        <v>-0.3293765187263489</v>
       </c>
       <c r="B79">
-        <v>0.4293619096279144</v>
+        <v>0.476565033197403</v>
       </c>
       <c r="C79">
-        <v>0.3083365559577942</v>
+        <v>0.3066969215869904</v>
       </c>
       <c r="D79">
-        <v>-0.3249997794628143</v>
+        <v>-0.3284972608089447</v>
       </c>
       <c r="E79">
-        <v>-0.0189109705388546</v>
+        <v>-0.02675222419202328</v>
       </c>
       <c r="F79">
-        <v>0.1331266462802887</v>
+        <v>0.1055681183934212</v>
       </c>
       <c r="G79">
-        <v>-0.5514201521873474</v>
+        <v>-0.5664631724357605</v>
       </c>
       <c r="H79">
-        <v>-0.1662336736917496</v>
+        <v>-0.1869361102581024</v>
       </c>
       <c r="I79">
-        <v>0.02384805679321289</v>
+        <v>0.03237782791256905</v>
       </c>
       <c r="J79">
-        <v>-0.3134702742099762</v>
+        <v>-0.3103361129760742</v>
       </c>
       <c r="K79">
-        <v>-0.06862148642539978</v>
+        <v>-0.07558674365282059</v>
       </c>
       <c r="L79">
-        <v>0.4133192896842957</v>
+        <v>0.4376231133937836</v>
       </c>
       <c r="M79">
         <v>-0.307576984167099</v>
       </c>
       <c r="N79">
-        <v>-0.119240865111351</v>
+        <v>-0.1114961504936218</v>
       </c>
       <c r="O79">
-        <v>0.2963194847106934</v>
+        <v>0.2765836417675018</v>
       </c>
       <c r="Q79">
-        <v>0.2222205102443695</v>
+        <v>0.2321176826953888</v>
       </c>
     </row>
     <row r="80" spans="1:17">
       <c r="A80">
-        <v>-0.4258958399295807</v>
+        <v>-0.4265842735767365</v>
       </c>
       <c r="B80">
-        <v>0.2121769785881042</v>
+        <v>0.2144017219543457</v>
       </c>
       <c r="C80">
-        <v>-0.2056613713502884</v>
+        <v>-0.2057618200778961</v>
       </c>
       <c r="D80">
-        <v>-0.4300251305103302</v>
+        <v>-0.4319955110549927</v>
       </c>
       <c r="E80">
-        <v>-0.1280908286571503</v>
+        <v>-0.1351667195558548</v>
       </c>
       <c r="F80">
-        <v>-0.02654630877077579</v>
+        <v>-0.03614004328846931</v>
       </c>
       <c r="G80">
-        <v>-0.0554208867251873</v>
+        <v>-0.05386674031615257</v>
       </c>
       <c r="H80">
-        <v>0.05240405723452568</v>
+        <v>0.052366703748703</v>
       </c>
       <c r="I80">
-        <v>-0.2302134335041046</v>
+        <v>-0.2424808740615845</v>
       </c>
       <c r="J80">
-        <v>-0.3642235100269318</v>
+        <v>-0.3398896157741547</v>
       </c>
       <c r="K80">
-        <v>-0.009902274236083031</v>
+        <v>-0.01103413011878729</v>
       </c>
       <c r="L80">
-        <v>-0.3091342449188232</v>
+        <v>-0.2903652787208557</v>
       </c>
       <c r="M80">
         <v>0.1553605496883392</v>
       </c>
       <c r="N80">
-        <v>0.3582347631454468</v>
+        <v>0.3553652763366699</v>
       </c>
       <c r="O80">
-        <v>-0.4536103308200836</v>
+        <v>-0.4581703245639801</v>
       </c>
       <c r="Q80">
-        <v>0.3427285552024841</v>
+        <v>0.3561437726020813</v>
       </c>
     </row>
     <row r="81" spans="1:17">
       <c r="A81">
-        <v>0.07276488840579987</v>
+        <v>0.0315963439643383</v>
       </c>
       <c r="B81">
-        <v>-0.2250027358531952</v>
+        <v>-0.2357958853244781</v>
       </c>
       <c r="C81">
-        <v>-0.08867082744836807</v>
+        <v>-0.09160308539867401</v>
       </c>
       <c r="D81">
-        <v>-0.2577169835567474</v>
+        <v>-0.2569515407085419</v>
       </c>
       <c r="E81">
-        <v>0.5165103673934937</v>
+        <v>0.5392221212387085</v>
       </c>
       <c r="F81">
-        <v>-0.3024182319641113</v>
+        <v>-0.2768535017967224</v>
       </c>
       <c r="G81">
-        <v>0.03495876118540764</v>
+        <v>0.0481485053896904</v>
       </c>
       <c r="H81">
-        <v>-0.2099776715040207</v>
+        <v>-0.2174509316682816</v>
       </c>
       <c r="I81">
-        <v>0.2358098030090332</v>
+        <v>0.2289891690015793</v>
       </c>
       <c r="J81">
-        <v>-0.3771644234657288</v>
+        <v>-0.3761457800865173</v>
       </c>
       <c r="K81">
-        <v>0.3204490542411804</v>
+        <v>0.322118729352951</v>
       </c>
       <c r="L81">
-        <v>-0.0828835666179657</v>
+        <v>-0.09719205647706985</v>
       </c>
       <c r="M81">
         <v>-0.2401893436908722</v>
       </c>
       <c r="N81">
-        <v>-0.5284062027931213</v>
+        <v>-0.5356746315956116</v>
       </c>
       <c r="O81">
-        <v>-0.1658241003751755</v>
+        <v>-0.1822235882282257</v>
       </c>
       <c r="Q81">
-        <v>0.3954979181289673</v>
+        <v>0.4040217995643616</v>
       </c>
     </row>
     <row r="82" spans="1:17">
       <c r="A82">
-        <v>0.219370573759079</v>
+        <v>0.1963709592819214</v>
       </c>
       <c r="B82">
-        <v>0.1896488219499588</v>
+        <v>0.178228884935379</v>
       </c>
       <c r="C82">
-        <v>0.4265377819538116</v>
+        <v>0.4296539723873138</v>
       </c>
       <c r="D82">
-        <v>0.3505602180957794</v>
+        <v>0.3526170551776886</v>
       </c>
       <c r="E82">
-        <v>-0.107234388589859</v>
+        <v>-0.1128744632005692</v>
       </c>
       <c r="F82">
-        <v>0.09566951543092728</v>
+        <v>0.07803994417190552</v>
       </c>
       <c r="G82">
-        <v>0.1715280115604401</v>
+        <v>0.169202595949173</v>
       </c>
       <c r="H82">
-        <v>0.257707953453064</v>
+        <v>0.306295245885849</v>
       </c>
       <c r="I82">
-        <v>0.4329014122486115</v>
+        <v>0.4309318661689758</v>
       </c>
       <c r="J82">
-        <v>0.1442333608865738</v>
+        <v>0.1455486118793488</v>
       </c>
       <c r="K82">
-        <v>-0.4932189285755157</v>
+        <v>-0.4936970472335815</v>
       </c>
       <c r="L82">
-        <v>-0.05314082652330399</v>
+        <v>-0.02925780601799488</v>
       </c>
       <c r="M82">
         <v>-0.2291760742664337</v>
       </c>
       <c r="N82">
-        <v>-0.2211585640907288</v>
+        <v>-0.2305065989494324</v>
       </c>
       <c r="O82">
-        <v>0.1807929128408432</v>
+        <v>0.1736873388290405</v>
       </c>
       <c r="Q82">
-        <v>-0.1259777545928955</v>
+        <v>-0.1332331299781799</v>
       </c>
     </row>
     <row r="83" spans="1:17">
       <c r="A83">
-        <v>-0.3574177622795105</v>
+        <v>-0.2928314805030823</v>
       </c>
       <c r="B83">
-        <v>-0.3200275599956512</v>
+        <v>-0.3383600413799286</v>
       </c>
       <c r="C83">
-        <v>0.1158265173435211</v>
+        <v>0.1085938215255737</v>
       </c>
       <c r="D83">
-        <v>0.06530576199293137</v>
+        <v>0.06188571453094482</v>
       </c>
       <c r="E83">
-        <v>0.2378414273262024</v>
+        <v>0.2303016781806946</v>
       </c>
       <c r="F83">
-        <v>-0.2525092661380768</v>
+        <v>-0.2914197146892548</v>
       </c>
       <c r="G83">
-        <v>0.04502728581428528</v>
+        <v>0.02464439533650875</v>
       </c>
       <c r="H83">
-        <v>0.3937470316886902</v>
+        <v>0.366177499294281</v>
       </c>
       <c r="I83">
-        <v>0.2047698795795441</v>
+        <v>0.2047439366579056</v>
       </c>
       <c r="J83">
-        <v>-0.3572776615619659</v>
+        <v>-0.3578521609306335</v>
       </c>
       <c r="K83">
-        <v>-0.5883187651634216</v>
+        <v>-0.5985519886016846</v>
       </c>
       <c r="L83">
-        <v>-0.05473917722702026</v>
+        <v>-0.01813581958413124</v>
       </c>
       <c r="M83">
         <v>0.2902656495571136</v>
       </c>
       <c r="N83">
-        <v>0.09471177309751511</v>
+        <v>0.08367439359426498</v>
       </c>
       <c r="O83">
-        <v>0.5498136878013611</v>
+        <v>0.54710453748703</v>
       </c>
       <c r="Q83">
-        <v>0.1374520808458328</v>
+        <v>0.1389505565166473</v>
       </c>
     </row>
     <row r="84" spans="1:17">
       <c r="A84">
-        <v>0.3480616211891174</v>
+        <v>0.2440914064645767</v>
       </c>
       <c r="B84">
-        <v>0.2416362017393112</v>
+        <v>0.2443727999925613</v>
       </c>
       <c r="C84">
-        <v>0.2977030873298645</v>
+        <v>0.3028194904327393</v>
       </c>
       <c r="D84">
-        <v>-0.3598847687244415</v>
+        <v>-0.3581280112266541</v>
       </c>
       <c r="E84">
-        <v>0.4261496365070343</v>
+        <v>0.4178614020347595</v>
       </c>
       <c r="F84">
-        <v>0.2538311779499054</v>
+        <v>0.2682206332683563</v>
       </c>
       <c r="G84">
-        <v>-0.05799183249473572</v>
+        <v>-0.07680822908878326</v>
       </c>
       <c r="H84">
-        <v>-0.03743653371930122</v>
+        <v>-0.04019258171319962</v>
       </c>
       <c r="I84">
-        <v>-0.03729071840643883</v>
+        <v>-0.03861143812537193</v>
       </c>
       <c r="J84">
-        <v>-0.2207255065441132</v>
+        <v>-0.216819241642952</v>
       </c>
       <c r="K84">
-        <v>-0.4339567720890045</v>
+        <v>-0.4270581305027008</v>
       </c>
       <c r="L84">
-        <v>0.2367603927850723</v>
+        <v>0.2674709856510162</v>
       </c>
       <c r="M84">
         <v>0.4107278883457184</v>
       </c>
       <c r="N84">
-        <v>-0.006532486528158188</v>
+        <v>-0.001220127800479531</v>
       </c>
       <c r="O84">
-        <v>0.1407382935285568</v>
+        <v>0.1247244700789452</v>
       </c>
       <c r="Q84">
-        <v>-0.2733394503593445</v>
+        <v>-0.2550675570964813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>